<commit_message>
corrected drive counts for create commands
</commit_message>
<xml_diff>
--- a/ZFS/zfs-draid-configs.xlsx
+++ b/ZFS/zfs-draid-configs.xlsx
@@ -100,6 +100,18 @@
         </r>
       </text>
     </comment>
+    <comment ref="M1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">This is the “free space” in the filesystem you can actually use, can vary with compression</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="N1" authorId="0">
       <text>
         <r>
@@ -114,6 +126,27 @@
       </text>
     </comment>
     <comment ref="N129" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">“12GB” as seen by OS; </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="18"/>
+            <color rgb="FF2FFF12"/>
+            <rFont val="Menlo-Regular"/>
+            <family val="0"/>
+          </rPr>
+          <t xml:space="preserve">12002390016 bytes </t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="N131" authorId="0">
       <text>
         <r>
           <rPr>
@@ -164,7 +197,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="409" uniqueCount="263">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="437" uniqueCount="289">
   <si>
     <t xml:space="preserve">ZFS DRAID configs</t>
   </si>
@@ -354,6 +387,9 @@
     <t xml:space="preserve">Copy ~7.3GB isos from UDF dvd mounted to zstd-3 DS - including sync - with no UNAVAIL</t>
   </si>
   <si>
+    <t xml:space="preserve">sd{b..m}</t>
+  </si>
+  <si>
     <t xml:space="preserve">draid1:14d:16c:1s</t>
   </si>
   <si>
@@ -518,6 +554,9 @@
     <t xml:space="preserve">6 with 0 vspare and 5 pspare + 1 UNAVAIL</t>
   </si>
   <si>
+    <t xml:space="preserve">sdz sday sdaz sdby sdcy</t>
+  </si>
+  <si>
     <t xml:space="preserve">draid2:5d:8c:1s</t>
   </si>
   <si>
@@ -532,7 +571,7 @@
     <t xml:space="preserve">5 with 4 vspares and 1 UNAVAIL</t>
   </si>
   <si>
-    <t xml:space="preserve">sd{b..y} sda{a..f}</t>
+    <t xml:space="preserve">sd{b..y} sda{a..h}</t>
   </si>
   <si>
     <t xml:space="preserve">3 with 2 vspares and 2 UNAVAIL</t>
@@ -543,7 +582,7 @@
   </si>
   <si>
     <t xml:space="preserve">sd{b..q} \
-sd{b..y} sda{a..g}</t>
+sd{r..y} sda{a..h}</t>
   </si>
   <si>
     <t xml:space="preserve">draid1:5d:8c:2s</t>
@@ -561,7 +600,7 @@
     <t xml:space="preserve">sd{b..i} \ 
 sd{j..q} \
 sd{r..y} \
-sda{a..g}</t>
+sda{a..h}</t>
   </si>
   <si>
     <t xml:space="preserve">draid2:26d:32c:4s</t>
@@ -895,6 +934,9 @@
     <t xml:space="preserve">draid2:12d:24c:2s</t>
   </si>
   <si>
+    <t xml:space="preserve">More data disks, less lost to parity, 1 vspare for every (12) disks</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <sz val="12"/>
@@ -932,6 +974,12 @@
   </si>
   <si>
     <t xml:space="preserve">draid2:12d:96c:12s</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Should be 14 with 12 vspares + 2 UNAVAIL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">More data disks, less lost to parity, 1 vspare for every (8) disks</t>
   </si>
   <si>
     <t xml:space="preserve">draid2:24d:96c:8s</t>
@@ -1195,6 +1243,115 @@
   </si>
   <si>
     <t xml:space="preserve">Disk size change</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DRAID2:5d:1s:8c</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">draid1:13d:16c:2s
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">draid1:13d:16c:2s</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">draid1:5d:8c:2s
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">draid1:5d:8c:2s
+draid1:5d:8c:2s
+draid1:5d:8c:2s</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">draid2:12d:16c:2s
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">draid2:12d:16c:2s</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">draid2:4d:8c:2s
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">draid2:4d:8c:2s
+draid2:4d:8c:2s
+draid2:4d:8c:2s</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">draid2:5d:8c:1s
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Courier New"/>
+        <family val="3"/>
+      </rPr>
+      <t xml:space="preserve">draid2:5d:8c:1s
+draid2:5d:8c:1s
+draid2:5d:8c:1s</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">Now this will really break your brain:</t>
@@ -1368,7 +1525,52 @@
     <t xml:space="preserve">Original Commit:</t>
   </si>
   <si>
+    <t xml:space="preserve">To deallocate a hotspare from the “spares” list:</t>
+  </si>
+  <si>
     <t xml:space="preserve">https://github.com/openzfs/zfs/pull/10102</t>
+  </si>
+  <si>
+    <t xml:space="preserve">zpool remove $zp sdX</t>
+  </si>
+  <si>
+    <t xml:space="preserve">( “detach” is wrong syntax )</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Utility - handy drive slicer:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://github.com/kneutron/ansitest/blob/master/ZFS/zfs-drive-slicer.sh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This would have made my life a lot easier had I created it earlier!</t>
+  </si>
+  <si>
+    <t xml:space="preserve">If you want it to look nice pipe output to ‘ column -t ‘</t>
+  </si>
+  <si>
+    <t xml:space="preserve">zfs-drive-slicer.sh 96 16 |column -t</t>
+  </si>
+  <si>
+    <t xml:space="preserve"># 16 per vdev = 6 vdevs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sdb   sdc   sdd   sde   sdf   sdg   sdh   sdi   sdj   sdk   sdl   sdm   sdn   sdo   sdp   sdq   \</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sdr   sds   sdt   sdu   sdv   sdw   sdx   sdy   sdaa  sdab  sdac  sdad  sdae  sdaf  sdag  sdah  \</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sdai  sdaj  sdak  sdal  sdam  sdan  sdao  sdap  sdaq  sdar  sdas  sdat  sdau  sdav  sdaw  sdax  \</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sdba  sdbb  sdbc  sdbd  sdbe  sdbf  sdbg  sdbh  sdbi  sdbj  sdbk  sdbl  sdbm  sdbn  sdbo  sdbp  \</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sdbq  sdbr  sdbs  sdbt  sdbu  sdbv  sdbw  sdbx  sdca  sdcb  sdcc  sdcd  sdce  sdcf  sdcg  sdch  \</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sdci  sdcj  sdck  sdcl  sdcm  sdcn  sdco  sdcp  sdcq  sdcr  sdcs  sdct  sdcu  sdcv  sdcw  sdcx  \</t>
   </si>
 </sst>
 </file>
@@ -1380,7 +1582,7 @@
     <numFmt numFmtId="165" formatCode="hh:mm"/>
     <numFmt numFmtId="166" formatCode="General"/>
   </numFmts>
-  <fonts count="27">
+  <fonts count="29">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1492,6 +1694,13 @@
     <font>
       <b val="true"/>
       <sz val="10"/>
+      <color rgb="FF00A933"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
@@ -1537,8 +1746,15 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b val="true"/>
+      <sz val="12"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1555,6 +1771,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF81D41A"/>
         <bgColor rgb="FF2FFF12"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFBF00"/>
+        <bgColor rgb="FFFF9900"/>
       </patternFill>
     </fill>
     <fill>
@@ -1598,7 +1820,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="70">
+  <cellXfs count="76">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1815,6 +2037,10 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="166" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="166" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1851,11 +2077,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="21" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1863,19 +2097,31 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="21" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="22" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="27" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1933,13 +2179,13 @@
       <rgbColor rgb="FF3366FF"/>
       <rgbColor rgb="FF33CCCC"/>
       <rgbColor rgb="FF81D41A"/>
-      <rgbColor rgb="FFFFCC00"/>
+      <rgbColor rgb="FFFFBF00"/>
       <rgbColor rgb="FFFF9900"/>
       <rgbColor rgb="FFFF4000"/>
       <rgbColor rgb="FF666699"/>
       <rgbColor rgb="FF969696"/>
       <rgbColor rgb="FF003366"/>
-      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF00A933"/>
       <rgbColor rgb="FF003300"/>
       <rgbColor rgb="FF333300"/>
       <rgbColor rgb="FFC9211E"/>
@@ -1956,12 +2202,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AMJ151"/>
+  <dimension ref="A1:AMJ153"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="I2" activeCellId="0" sqref="I2"/>
+      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2733,7 +2979,7 @@
         <v>draid1:10d:12c:1s</v>
       </c>
       <c r="U15" s="16" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2752,7 +2998,7 @@
     </row>
     <row r="17" customFormat="false" ht="34.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="21" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B17" s="2" t="n">
         <v>16</v>
@@ -2780,7 +3026,7 @@
         <v>23</v>
       </c>
       <c r="J17" s="20" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="K17" s="7"/>
       <c r="L17" s="2" t="n">
@@ -2812,7 +3058,7 @@
         <v>draid1:14d:16c:1s</v>
       </c>
       <c r="U17" s="16" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="45.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2844,7 +3090,7 @@
       <c r="H19" s="19"/>
       <c r="I19" s="20"/>
       <c r="J19" s="2" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="K19" s="30" t="n">
         <v>0.0770833333333333</v>
@@ -2857,7 +3103,7 @@
     </row>
     <row r="20" customFormat="false" ht="23.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="21" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B20" s="2" t="n">
         <v>16</v>
@@ -2882,10 +3128,10 @@
         <v>1</v>
       </c>
       <c r="I20" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="J20" s="20" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="K20" s="7"/>
       <c r="L20" s="2" t="n">
@@ -2920,13 +3166,13 @@
         <v>draid1:13d:16c:2s</v>
       </c>
       <c r="U20" s="16" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="V20" s="0" t="s">
         <v>26</v>
       </c>
       <c r="W20" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="45.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2959,7 +3205,7 @@
         <v>23</v>
       </c>
       <c r="J21" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="K21" s="7" t="n">
         <v>0.0319444444444444</v>
@@ -2989,14 +3235,10 @@
         <v>16</v>
       </c>
       <c r="T21" s="23" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="U21" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="V21" s="0" t="n">
-        <f aca="false">G21</f>
-        <v>0</v>
+        <v>65</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="45.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3006,7 +3248,7 @@
       <c r="G22" s="26"/>
       <c r="I22" s="20"/>
       <c r="J22" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="K22" s="34" t="n">
         <v>0.05625</v>
@@ -3028,7 +3270,7 @@
       <c r="G23" s="26"/>
       <c r="I23" s="20"/>
       <c r="J23" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="K23" s="34" t="n">
         <v>0.110416666666667</v>
@@ -3045,7 +3287,7 @@
     </row>
     <row r="24" s="17" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="21" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B24" s="2" t="n">
         <v>16</v>
@@ -3070,10 +3312,10 @@
         <v>2</v>
       </c>
       <c r="I24" s="13" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="J24" s="20" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="K24" s="7"/>
       <c r="L24" s="2" t="n">
@@ -3106,7 +3348,7 @@
         <v>draid2:13d:16c:1s</v>
       </c>
       <c r="U24" s="16" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="V24" s="0"/>
       <c r="AMJ24" s="0"/>
@@ -3150,7 +3392,7 @@
     </row>
     <row r="27" customFormat="false" ht="34.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B27" s="2" t="n">
         <v>24</v>
@@ -3178,7 +3420,7 @@
         <v>23</v>
       </c>
       <c r="J27" s="2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="K27" s="7" t="n">
         <v>0.0243055555555556</v>
@@ -3215,12 +3457,12 @@
         <v>draid1:8d:24c:1s</v>
       </c>
       <c r="U27" s="16" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="34.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B28" s="2" t="n">
         <v>24</v>
@@ -3245,10 +3487,10 @@
         <v>1</v>
       </c>
       <c r="I28" s="20" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="J28" s="2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="K28" s="7" t="n">
         <v>0.0222222222222222</v>
@@ -3278,10 +3520,10 @@
         <v>24</v>
       </c>
       <c r="T28" s="23" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="U28" s="23" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="56.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3290,7 +3532,7 @@
       <c r="F29" s="25"/>
       <c r="H29" s="19"/>
       <c r="J29" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="K29" s="31" t="n">
         <v>0.0194444444444444</v>
@@ -3308,7 +3550,7 @@
       <c r="H30" s="19"/>
       <c r="I30" s="25"/>
       <c r="J30" s="2" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="K30" s="7" t="n">
         <v>0.0201388888888889</v>
@@ -3325,7 +3567,7 @@
       <c r="F31" s="25"/>
       <c r="H31" s="19"/>
       <c r="J31" s="2" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="K31" s="31" t="n">
         <v>0.0138888888888889</v>
@@ -3351,7 +3593,7 @@
     </row>
     <row r="33" customFormat="false" ht="34.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="21" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B33" s="2" t="n">
         <v>24</v>
@@ -3376,10 +3618,10 @@
         <v>2</v>
       </c>
       <c r="I33" s="20" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="J33" s="2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="K33" s="7" t="n">
         <v>0.0263888888888889</v>
@@ -3412,10 +3654,10 @@
         <v>24</v>
       </c>
       <c r="T33" s="23" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="U33" s="23" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="45.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3425,7 +3667,7 @@
       <c r="F34" s="25"/>
       <c r="H34" s="19"/>
       <c r="J34" s="2" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="K34" s="31" t="n">
         <v>0.0166666666666667</v>
@@ -3443,7 +3685,7 @@
       <c r="F35" s="25"/>
       <c r="H35" s="19"/>
       <c r="J35" s="20" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="K35" s="31" t="n">
         <v>0.00902777777777778</v>
@@ -3515,7 +3757,7 @@
         <v>23</v>
       </c>
       <c r="J38" s="2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="K38" s="7" t="n">
         <v>0.0243055555555556</v>
@@ -3545,16 +3787,16 @@
         <v>25</v>
       </c>
       <c r="T38" s="23" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="U38" s="23" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="V38" s="0" t="s">
         <v>26</v>
       </c>
       <c r="W38" s="0" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="45.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3563,7 +3805,7 @@
       <c r="F39" s="25"/>
       <c r="H39" s="19"/>
       <c r="J39" s="2" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="K39" s="31" t="n">
         <v>0.01875</v>
@@ -3578,7 +3820,7 @@
       <c r="F40" s="25"/>
       <c r="H40" s="19"/>
       <c r="J40" s="41" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="K40" s="31" t="n">
         <v>0.0194444444444444</v>
@@ -3593,7 +3835,7 @@
       <c r="F41" s="25"/>
       <c r="H41" s="19"/>
       <c r="J41" s="2" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="K41" s="42" t="n">
         <v>0.0368055555555556</v>
@@ -3615,7 +3857,7 @@
     </row>
     <row r="43" customFormat="false" ht="40.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="43" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B43" s="1" t="n">
         <v>24</v>
@@ -3668,16 +3910,16 @@
         <v>25</v>
       </c>
       <c r="T43" s="23" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="U43" s="23" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="V43" s="0" t="s">
         <v>26</v>
       </c>
       <c r="W43" s="0" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3716,7 +3958,7 @@
         <v>23</v>
       </c>
       <c r="J45" s="2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="K45" s="7" t="n">
         <v>0.0236111111111111</v>
@@ -3746,22 +3988,22 @@
         <v>25</v>
       </c>
       <c r="T45" s="23" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="U45" s="23" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="V45" s="0" t="s">
         <v>26</v>
       </c>
       <c r="W45" s="0" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="45.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F46" s="25"/>
       <c r="J46" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="K46" s="31" t="n">
         <v>0.0173611111111111</v>
@@ -3772,7 +4014,7 @@
     <row r="47" customFormat="false" ht="45.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F47" s="25"/>
       <c r="J47" s="41" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="K47" s="31" t="n">
         <v>0.0104166666666667</v>
@@ -3788,7 +4030,7 @@
     </row>
     <row r="49" customFormat="false" ht="54.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="21" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B49" s="1" t="n">
         <v>24</v>
@@ -3813,10 +4055,10 @@
         <v>2</v>
       </c>
       <c r="I49" s="20" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="J49" s="2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="K49" s="7" t="n">
         <v>0.0361111111111111</v>
@@ -3849,10 +4091,10 @@
         <v>24</v>
       </c>
       <c r="T49" s="23" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="U49" s="23" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="V49" s="0" t="n">
         <f aca="false">G49</f>
@@ -3866,7 +4108,7 @@
       <c r="G50" s="45"/>
       <c r="H50" s="19"/>
       <c r="J50" s="2" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="K50" s="31" t="n">
         <v>0.0298611111111111</v>
@@ -3882,7 +4124,7 @@
       <c r="G51" s="45"/>
       <c r="H51" s="19"/>
       <c r="J51" s="41" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="K51" s="31" t="n">
         <v>0.0166666666666667</v>
@@ -3904,7 +4146,7 @@
     </row>
     <row r="53" customFormat="false" ht="23.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="44" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B53" s="1" t="n">
         <v>24</v>
@@ -3929,7 +4171,7 @@
         <v>1</v>
       </c>
       <c r="I53" s="20" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="J53" s="2"/>
       <c r="K53" s="0"/>
@@ -3962,11 +4204,13 @@
         <v>draid1:8d:24c:0s</v>
       </c>
       <c r="U53" s="16" t="s">
-        <v>72</v>
-      </c>
-      <c r="V53" s="0" t="n">
-        <f aca="false">G53</f>
-        <v>5</v>
+        <v>73</v>
+      </c>
+      <c r="V53" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="W53" s="0" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3978,7 +4222,7 @@
     </row>
     <row r="55" customFormat="false" ht="40.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="1" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="B55" s="49" t="n">
         <v>24</v>
@@ -4031,16 +4275,16 @@
         <v>25</v>
       </c>
       <c r="T55" s="23" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="U55" s="23" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="V55" s="0" t="s">
         <v>26</v>
       </c>
       <c r="W55" s="0" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4067,7 +4311,7 @@
     </row>
     <row r="58" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="21" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="B58" s="21" t="n">
         <v>32</v>
@@ -4092,10 +4336,10 @@
         <v>1</v>
       </c>
       <c r="I58" s="2" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="J58" s="17" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="K58" s="17"/>
       <c r="L58" s="1" t="n">
@@ -4130,12 +4374,12 @@
         <v>draid1:27d:32c:4s</v>
       </c>
       <c r="U58" s="16" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="27.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B59" s="21" t="n">
         <v>32</v>
@@ -4160,7 +4404,7 @@
         <v>1</v>
       </c>
       <c r="I59" s="2" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="J59" s="17"/>
       <c r="K59" s="17"/>
@@ -4189,15 +4433,15 @@
         <v>32</v>
       </c>
       <c r="T59" s="23" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="U59" s="23" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="54.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="45" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="B60" s="21" t="n">
         <v>32</v>
@@ -4222,10 +4466,10 @@
         <v>1</v>
       </c>
       <c r="I60" s="2" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="J60" s="17" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="K60" s="17"/>
       <c r="L60" s="44" t="n">
@@ -4253,15 +4497,15 @@
         <v>32</v>
       </c>
       <c r="T60" s="23" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="U60" s="23" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="1" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="B61" s="21" t="n">
         <v>32</v>
@@ -4286,10 +4530,10 @@
         <v>2</v>
       </c>
       <c r="I61" s="2" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="J61" s="17" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="K61" s="17"/>
       <c r="L61" s="1" t="n">
@@ -4321,12 +4565,12 @@
         <v>draid2:26d:32c:4s</v>
       </c>
       <c r="U61" s="16" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="27.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="1" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="B62" s="21" t="n">
         <v>32</v>
@@ -4351,7 +4595,7 @@
         <v>2</v>
       </c>
       <c r="I62" s="2" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="J62" s="17"/>
       <c r="K62" s="17"/>
@@ -4380,15 +4624,15 @@
         <v>32</v>
       </c>
       <c r="T62" s="23" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="U62" s="23" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="54.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A63" s="45" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="B63" s="21" t="n">
         <v>32</v>
@@ -4413,10 +4657,10 @@
         <v>2</v>
       </c>
       <c r="I63" s="2" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="J63" s="17" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="K63" s="17"/>
       <c r="L63" s="21" t="n">
@@ -4444,19 +4688,15 @@
         <v>32</v>
       </c>
       <c r="T63" s="23" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="U63" s="23" t="s">
-        <v>113</v>
-      </c>
-      <c r="V63" s="0" t="n">
-        <f aca="false">G63</f>
-        <v>0</v>
+        <v>115</v>
       </c>
     </row>
     <row r="64" s="17" customFormat="true" ht="54.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A64" s="21" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="B64" s="21" t="n">
         <v>32</v>
@@ -4481,10 +4721,10 @@
         <v>2</v>
       </c>
       <c r="I64" s="20" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="J64" s="17" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="L64" s="21" t="n">
         <v>102</v>
@@ -4516,12 +4756,9 @@
         <v>draid2:5d:8c:1s</v>
       </c>
       <c r="U64" s="23" t="s">
-        <v>113</v>
-      </c>
-      <c r="V64" s="0" t="n">
-        <f aca="false">G64</f>
-        <v>0</v>
-      </c>
+        <v>115</v>
+      </c>
+      <c r="V64" s="0"/>
       <c r="AMJ64" s="0"/>
     </row>
     <row r="65" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4532,10 +4769,6 @@
       <c r="Q65" s="18"/>
       <c r="T65" s="16"/>
       <c r="U65" s="16"/>
-      <c r="V65" s="0" t="n">
-        <f aca="false">G65</f>
-        <v>0</v>
-      </c>
     </row>
     <row r="66" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B66" s="21"/>
@@ -4545,14 +4778,10 @@
       <c r="Q66" s="18"/>
       <c r="T66" s="16"/>
       <c r="U66" s="16"/>
-      <c r="V66" s="0" t="n">
-        <f aca="false">G66</f>
-        <v>0</v>
-      </c>
     </row>
     <row r="67" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A67" s="1" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="B67" s="21" t="n">
         <v>48</v>
@@ -4608,19 +4837,15 @@
         <v>24</v>
       </c>
       <c r="T67" s="16" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="U67" s="16" t="s">
-        <v>125</v>
-      </c>
-      <c r="V67" s="0" t="n">
-        <f aca="false">G67</f>
-        <v>0</v>
+        <v>127</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="27.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A68" s="1" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B68" s="21" t="n">
         <v>48</v>
@@ -4645,7 +4870,7 @@
         <v>1</v>
       </c>
       <c r="I68" s="2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="K68" s="0"/>
       <c r="L68" s="1" t="n">
@@ -4673,19 +4898,15 @@
         <v>48</v>
       </c>
       <c r="T68" s="23" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="U68" s="23" t="s">
-        <v>127</v>
-      </c>
-      <c r="V68" s="0" t="n">
-        <f aca="false">G68</f>
-        <v>0</v>
+        <v>129</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="40.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A69" s="1" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="B69" s="21" t="n">
         <v>48</v>
@@ -4710,7 +4931,7 @@
         <v>1</v>
       </c>
       <c r="I69" s="2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="K69" s="0"/>
       <c r="L69" s="1" t="n">
@@ -4738,10 +4959,10 @@
         <v>48</v>
       </c>
       <c r="T69" s="23" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="U69" s="23" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4756,7 +4977,7 @@
     </row>
     <row r="71" customFormat="false" ht="45.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A71" s="21" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="B71" s="21" t="n">
         <v>48</v>
@@ -4781,10 +5002,10 @@
         <v>2</v>
       </c>
       <c r="I71" s="2" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="J71" s="2" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="K71" s="7" t="n">
         <v>0.0430555555555556</v>
@@ -4818,7 +5039,7 @@
         <v>draid2:8d:48c:2s</v>
       </c>
       <c r="U71" s="16" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="56.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4828,7 +5049,7 @@
       <c r="G72" s="21"/>
       <c r="H72" s="19"/>
       <c r="J72" s="2" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="K72" s="31" t="n">
         <v>0.0333333333333333</v>
@@ -4839,7 +5060,7 @@
     </row>
     <row r="73" customFormat="false" ht="27.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A73" s="1" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="B73" s="21" t="n">
         <v>48</v>
@@ -4864,7 +5085,7 @@
         <v>2</v>
       </c>
       <c r="I73" s="2" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="K73" s="0"/>
       <c r="L73" s="1" t="n">
@@ -4895,10 +5116,10 @@
         <v>24</v>
       </c>
       <c r="T73" s="23" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="U73" s="23" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -4913,7 +5134,7 @@
     </row>
     <row r="75" customFormat="false" ht="40.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A75" s="1" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="B75" s="21" t="n">
         <v>48</v>
@@ -4938,7 +5159,7 @@
         <v>2</v>
       </c>
       <c r="I75" s="2" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="K75" s="0"/>
       <c r="L75" s="1" t="n">
@@ -4966,15 +5187,15 @@
         <v>48</v>
       </c>
       <c r="T75" s="23" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="U75" s="23" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
     </row>
     <row r="76" s="17" customFormat="true" ht="40.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="21" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="B76" s="21" t="n">
         <v>48</v>
@@ -4999,10 +5220,10 @@
         <v>2</v>
       </c>
       <c r="I76" s="2" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="J76" s="2" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="L76" s="1" t="n">
         <v>153</v>
@@ -5034,7 +5255,7 @@
         <v>draid2:12d:16c:2s</v>
       </c>
       <c r="U76" s="23" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="V76" s="0"/>
       <c r="AMJ76" s="0"/>
@@ -5059,7 +5280,7 @@
     </row>
     <row r="79" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A79" s="1" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="B79" s="21" t="n">
         <v>72</v>
@@ -5119,12 +5340,12 @@
         <v>draid1:8d:72c:2s</v>
       </c>
       <c r="U79" s="16" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="27.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="1" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="B80" s="21" t="n">
         <v>72</v>
@@ -5177,10 +5398,10 @@
         <v>72</v>
       </c>
       <c r="T80" s="23" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="U80" s="23" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5195,7 +5416,7 @@
     </row>
     <row r="82" customFormat="false" ht="40.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A82" s="1" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="B82" s="21" t="n">
         <v>72</v>
@@ -5248,15 +5469,15 @@
         <v>72</v>
       </c>
       <c r="T82" s="23" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="U82" s="23" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
     </row>
     <row r="83" s="17" customFormat="true" ht="40.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A83" s="21" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="B83" s="21" t="n">
         <v>72</v>
@@ -5284,7 +5505,7 @@
         <v>44</v>
       </c>
       <c r="J83" s="2" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="L83" s="1" t="n">
         <v>241</v>
@@ -5312,10 +5533,10 @@
       </c>
       <c r="S83" s="5"/>
       <c r="T83" s="23" t="s">
+        <v>151</v>
+      </c>
+      <c r="U83" s="23" t="s">
         <v>149</v>
-      </c>
-      <c r="U83" s="23" t="s">
-        <v>147</v>
       </c>
       <c r="V83" s="0"/>
       <c r="AMJ83" s="0"/>
@@ -5331,7 +5552,7 @@
       <c r="H84" s="19"/>
       <c r="I84" s="2"/>
       <c r="J84" s="2" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="K84" s="31" t="n">
         <v>0.0340277777777778</v>
@@ -5360,7 +5581,7 @@
       <c r="H85" s="19"/>
       <c r="I85" s="2"/>
       <c r="J85" s="2" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="K85" s="31" t="n">
         <v>0.0354166666666667</v>
@@ -5390,7 +5611,7 @@
     </row>
     <row r="87" customFormat="false" ht="23.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A87" s="21" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="B87" s="21" t="n">
         <v>72</v>
@@ -5415,10 +5636,10 @@
         <v>2</v>
       </c>
       <c r="I87" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="J87" s="20" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="K87" s="0"/>
       <c r="L87" s="1" t="n">
@@ -5453,12 +5674,12 @@
         <v>draid2:12d:72c:2s</v>
       </c>
       <c r="U87" s="16" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
     </row>
     <row r="88" s="17" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A88" s="21" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="B88" s="21" t="n">
         <v>72</v>
@@ -5483,10 +5704,10 @@
         <v>2</v>
       </c>
       <c r="I88" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="J88" s="2" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="L88" s="1" t="n">
         <v>256</v>
@@ -5518,7 +5739,7 @@
         <v>draid2:8d:72c:2s</v>
       </c>
       <c r="U88" s="16" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="V88" s="0"/>
       <c r="AMJ88" s="0"/>
@@ -5549,7 +5770,7 @@
     </row>
     <row r="90" customFormat="false" ht="27.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A90" s="49" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="B90" s="21" t="n">
         <v>72</v>
@@ -5574,7 +5795,7 @@
         <v>2</v>
       </c>
       <c r="I90" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="K90" s="0"/>
       <c r="L90" s="1" t="n">
@@ -5602,15 +5823,15 @@
         <v>72</v>
       </c>
       <c r="T90" s="23" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="U90" s="23" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
     </row>
     <row r="91" s="17" customFormat="true" ht="27.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A91" s="21" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="B91" s="21" t="n">
         <v>72</v>
@@ -5635,10 +5856,10 @@
         <v>2</v>
       </c>
       <c r="I91" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="J91" s="17" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="L91" s="1" t="n">
         <v>248</v>
@@ -5666,17 +5887,17 @@
       </c>
       <c r="S91" s="5"/>
       <c r="T91" s="23" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="U91" s="23" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="V91" s="0"/>
       <c r="AMJ91" s="0"/>
     </row>
     <row r="92" s="17" customFormat="true" ht="27.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A92" s="21" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="B92" s="21" t="n">
         <v>72</v>
@@ -5701,10 +5922,10 @@
         <v>2</v>
       </c>
       <c r="I92" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="J92" s="2" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="L92" s="1" t="n">
         <v>248</v>
@@ -5732,10 +5953,10 @@
       </c>
       <c r="S92" s="5"/>
       <c r="T92" s="23" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="U92" s="23" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="V92" s="0"/>
       <c r="AMJ92" s="0"/>
@@ -5753,7 +5974,7 @@
     </row>
     <row r="94" customFormat="false" ht="40.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="1" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="B94" s="21" t="n">
         <v>72</v>
@@ -5778,10 +5999,10 @@
         <v>2</v>
       </c>
       <c r="I94" s="2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="J94" s="2" t="s">
-        <v>139</v>
+        <v>165</v>
       </c>
       <c r="K94" s="0"/>
       <c r="L94" s="1" t="n">
@@ -5809,10 +6030,10 @@
         <v>72</v>
       </c>
       <c r="T94" s="23" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="U94" s="23" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5836,7 +6057,7 @@
     </row>
     <row r="97" customFormat="false" ht="23.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A97" s="21" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="B97" s="21" t="n">
         <v>96</v>
@@ -5850,7 +6071,7 @@
       <c r="E97" s="21" t="n">
         <v>6</v>
       </c>
-      <c r="F97" s="25" t="n">
+      <c r="F97" s="54" t="n">
         <f aca="false">E97*C97</f>
         <v>6</v>
       </c>
@@ -5861,7 +6082,7 @@
         <v>2</v>
       </c>
       <c r="I97" s="20" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="J97" s="2"/>
       <c r="K97" s="0"/>
@@ -5881,7 +6102,7 @@
         <f aca="false">N97*B97</f>
         <v>358.08</v>
       </c>
-      <c r="Q97" s="54" t="n">
+      <c r="Q97" s="55" t="n">
         <f aca="false">P97-M97</f>
         <v>103.08</v>
       </c>
@@ -5897,27 +6118,27 @@
         <v>draid2:8d:96c:6s</v>
       </c>
       <c r="U97" s="16" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="V97" s="0" t="s">
         <v>26</v>
       </c>
       <c r="W97" s="0" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="45.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F98" s="25"/>
       <c r="I98" s="2" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="K98" s="0"/>
       <c r="T98" s="16"/>
       <c r="U98" s="16"/>
     </row>
-    <row r="99" s="17" customFormat="true" ht="23.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="99" s="17" customFormat="true" ht="34.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A99" s="21" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="B99" s="21" t="n">
         <v>96</v>
@@ -5941,9 +6162,11 @@
       <c r="H99" s="50" t="n">
         <v>2</v>
       </c>
-      <c r="I99" s="20"/>
+      <c r="I99" s="20" t="s">
+        <v>173</v>
+      </c>
       <c r="J99" s="2" t="s">
-        <v>139</v>
+        <v>174</v>
       </c>
       <c r="L99" s="1" t="n">
         <v>308</v>
@@ -5961,7 +6184,7 @@
         <f aca="false">N99*B99</f>
         <v>358.08</v>
       </c>
-      <c r="Q99" s="54" t="n">
+      <c r="Q99" s="55" t="n">
         <f aca="false">P99-M99</f>
         <v>110.08</v>
       </c>
@@ -5975,14 +6198,14 @@
         <v>draid2:12d:96c:12s</v>
       </c>
       <c r="U99" s="16" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="V99" s="0"/>
       <c r="AMJ99" s="0"/>
     </row>
     <row r="100" s="17" customFormat="true" ht="23.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="21" t="s">
-        <v>170</v>
+        <v>175</v>
       </c>
       <c r="B100" s="21" t="n">
         <v>96</v>
@@ -6007,10 +6230,10 @@
         <v>2</v>
       </c>
       <c r="I100" s="20" t="s">
-        <v>171</v>
+        <v>176</v>
       </c>
       <c r="J100" s="20" t="s">
-        <v>172</v>
+        <v>177</v>
       </c>
       <c r="L100" s="21" t="n">
         <v>322</v>
@@ -6028,7 +6251,7 @@
         <f aca="false">N100*B100</f>
         <v>358.08</v>
       </c>
-      <c r="Q100" s="55" t="n">
+      <c r="Q100" s="56" t="n">
         <f aca="false">P100-M100</f>
         <v>79.08</v>
       </c>
@@ -6042,7 +6265,7 @@
         <v>draid2:24d:96c:8s</v>
       </c>
       <c r="U100" s="16" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="V100" s="0"/>
       <c r="AMJ100" s="0"/>
@@ -6058,7 +6281,7 @@
       <c r="H101" s="35"/>
       <c r="I101" s="20"/>
       <c r="J101" s="2" t="s">
-        <v>173</v>
+        <v>178</v>
       </c>
       <c r="K101" s="31" t="n">
         <v>0.0347222222222222</v>
@@ -6068,7 +6291,7 @@
       <c r="N101" s="1"/>
       <c r="O101" s="1"/>
       <c r="P101" s="1"/>
-      <c r="Q101" s="55"/>
+      <c r="Q101" s="56"/>
       <c r="R101" s="1"/>
       <c r="S101" s="5"/>
       <c r="T101" s="16"/>
@@ -6087,7 +6310,7 @@
       <c r="H102" s="35"/>
       <c r="I102" s="20"/>
       <c r="J102" s="2" t="s">
-        <v>174</v>
+        <v>179</v>
       </c>
       <c r="K102" s="31" t="n">
         <v>0.0243055555555556</v>
@@ -6097,7 +6320,7 @@
       <c r="N102" s="1"/>
       <c r="O102" s="1"/>
       <c r="P102" s="1"/>
-      <c r="Q102" s="55"/>
+      <c r="Q102" s="56"/>
       <c r="R102" s="1"/>
       <c r="S102" s="5"/>
       <c r="T102" s="16"/>
@@ -6114,7 +6337,7 @@
     </row>
     <row r="104" customFormat="false" ht="34.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A104" s="21" t="s">
-        <v>175</v>
+        <v>180</v>
       </c>
       <c r="B104" s="1" t="n">
         <v>96</v>
@@ -6126,7 +6349,7 @@
         <v>48</v>
       </c>
       <c r="E104" s="2" t="s">
-        <v>176</v>
+        <v>181</v>
       </c>
       <c r="F104" s="33" t="n">
         <v>8</v>
@@ -6138,10 +6361,10 @@
         <v>2</v>
       </c>
       <c r="I104" s="20" t="s">
-        <v>177</v>
+        <v>182</v>
       </c>
       <c r="J104" s="2" t="s">
-        <v>178</v>
+        <v>183</v>
       </c>
       <c r="K104" s="0"/>
       <c r="L104" s="1" t="n">
@@ -6160,7 +6383,7 @@
         <f aca="false">N104*B104</f>
         <v>358.08</v>
       </c>
-      <c r="Q104" s="54" t="n">
+      <c r="Q104" s="55" t="n">
         <f aca="false">P104-M104</f>
         <v>109.08</v>
       </c>
@@ -6172,14 +6395,10 @@
         <v>24</v>
       </c>
       <c r="T104" s="23" t="s">
-        <v>179</v>
+        <v>184</v>
       </c>
       <c r="U104" s="23" t="s">
-        <v>180</v>
-      </c>
-      <c r="V104" s="0" t="n">
-        <f aca="false">G104</f>
-        <v>0</v>
+        <v>185</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6191,7 +6410,7 @@
     </row>
     <row r="106" customFormat="false" ht="54.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A106" s="21" t="s">
-        <v>181</v>
+        <v>186</v>
       </c>
       <c r="B106" s="1" t="n">
         <v>96</v>
@@ -6216,10 +6435,10 @@
         <v>2</v>
       </c>
       <c r="I106" s="2" t="s">
-        <v>182</v>
+        <v>187</v>
       </c>
       <c r="J106" s="2" t="s">
-        <v>183</v>
+        <v>188</v>
       </c>
       <c r="K106" s="0"/>
       <c r="L106" s="1" t="n">
@@ -6238,7 +6457,7 @@
         <f aca="false">N106*B106</f>
         <v>358.08</v>
       </c>
-      <c r="Q106" s="54" t="n">
+      <c r="Q106" s="55" t="n">
         <f aca="false">P106-M106</f>
         <v>120.08</v>
       </c>
@@ -6247,24 +6466,24 @@
         <v>100</v>
       </c>
       <c r="T106" s="23" t="s">
-        <v>184</v>
+        <v>189</v>
       </c>
       <c r="U106" s="23" t="s">
-        <v>185</v>
+        <v>190</v>
       </c>
       <c r="V106" s="0" t="s">
         <v>26</v>
       </c>
       <c r="W106" s="0" t="s">
-        <v>186</v>
+        <v>191</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="23.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F107" s="25"/>
       <c r="J107" s="2" t="s">
-        <v>187</v>
-      </c>
-      <c r="K107" s="56" t="n">
+        <v>192</v>
+      </c>
+      <c r="K107" s="57" t="n">
         <v>0.107638888888889</v>
       </c>
       <c r="T107" s="16"/>
@@ -6273,9 +6492,9 @@
     <row r="108" customFormat="false" ht="34.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F108" s="25"/>
       <c r="J108" s="2" t="s">
-        <v>188</v>
-      </c>
-      <c r="K108" s="57" t="n">
+        <v>193</v>
+      </c>
+      <c r="K108" s="58" t="n">
         <v>0.0756944444444444</v>
       </c>
       <c r="T108" s="16"/>
@@ -6284,9 +6503,9 @@
     <row r="109" customFormat="false" ht="34.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F109" s="25"/>
       <c r="J109" s="2" t="s">
-        <v>189</v>
-      </c>
-      <c r="K109" s="58" t="n">
+        <v>194</v>
+      </c>
+      <c r="K109" s="59" t="n">
         <v>0.0583333333333333</v>
       </c>
       <c r="T109" s="16"/>
@@ -6295,9 +6514,9 @@
     <row r="110" customFormat="false" ht="45.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F110" s="25"/>
       <c r="J110" s="2" t="s">
-        <v>190</v>
-      </c>
-      <c r="K110" s="58" t="n">
+        <v>195</v>
+      </c>
+      <c r="K110" s="59" t="n">
         <v>0.0569444444444444</v>
       </c>
       <c r="T110" s="16"/>
@@ -6306,17 +6525,17 @@
     <row r="111" customFormat="false" ht="45.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F111" s="25"/>
       <c r="J111" s="2" t="s">
-        <v>191</v>
-      </c>
-      <c r="K111" s="58" t="n">
+        <v>196</v>
+      </c>
+      <c r="K111" s="59" t="n">
         <v>0.00972222222222222</v>
       </c>
       <c r="T111" s="16"/>
       <c r="U111" s="16"/>
     </row>
     <row r="112" customFormat="false" ht="54.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A112" s="59" t="s">
-        <v>192</v>
+      <c r="A112" s="60" t="s">
+        <v>197</v>
       </c>
       <c r="B112" s="1" t="n">
         <v>96</v>
@@ -6328,7 +6547,7 @@
         <v>24</v>
       </c>
       <c r="E112" s="2" t="s">
-        <v>176</v>
+        <v>181</v>
       </c>
       <c r="F112" s="27" t="n">
         <v>16</v>
@@ -6340,10 +6559,10 @@
         <v>1</v>
       </c>
       <c r="I112" s="2" t="s">
-        <v>193</v>
+        <v>198</v>
       </c>
       <c r="J112" s="2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="K112" s="3" t="n">
         <v>0.0243055555555556</v>
@@ -6364,7 +6583,7 @@
         <f aca="false">N112*B112</f>
         <v>358.08</v>
       </c>
-      <c r="Q112" s="54" t="n">
+      <c r="Q112" s="55" t="n">
         <f aca="false">P112-M112</f>
         <v>107.08</v>
       </c>
@@ -6376,16 +6595,16 @@
         <v>24</v>
       </c>
       <c r="T112" s="23" t="s">
-        <v>194</v>
+        <v>199</v>
       </c>
       <c r="U112" s="23" t="s">
-        <v>185</v>
+        <v>190</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="34.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F113" s="25"/>
       <c r="J113" s="2" t="s">
-        <v>195</v>
+        <v>200</v>
       </c>
       <c r="K113" s="3" t="n">
         <v>0.0444444444444444</v>
@@ -6396,9 +6615,9 @@
     <row r="114" customFormat="false" ht="34.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F114" s="25"/>
       <c r="J114" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="K114" s="60" t="n">
+        <v>201</v>
+      </c>
+      <c r="K114" s="61" t="n">
         <v>0.0625</v>
       </c>
       <c r="T114" s="16"/>
@@ -6407,9 +6626,9 @@
     <row r="115" customFormat="false" ht="45.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="F115" s="25"/>
       <c r="J115" s="2" t="s">
-        <v>197</v>
-      </c>
-      <c r="K115" s="58" t="n">
+        <v>202</v>
+      </c>
+      <c r="K115" s="59" t="n">
         <v>0.0215277777777778</v>
       </c>
       <c r="T115" s="16"/>
@@ -6417,7 +6636,7 @@
     </row>
     <row r="116" s="17" customFormat="true" ht="54.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A116" s="21" t="s">
-        <v>198</v>
+        <v>203</v>
       </c>
       <c r="B116" s="1" t="n">
         <v>96</v>
@@ -6442,10 +6661,10 @@
         <v>1</v>
       </c>
       <c r="I116" s="2" t="s">
-        <v>193</v>
+        <v>198</v>
       </c>
       <c r="J116" s="2" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="K116" s="3"/>
       <c r="L116" s="1" t="n">
@@ -6464,7 +6683,7 @@
         <f aca="false">N116*B116</f>
         <v>358.08</v>
       </c>
-      <c r="Q116" s="55" t="n">
+      <c r="Q116" s="56" t="n">
         <f aca="false">P116-M116</f>
         <v>104.08</v>
       </c>
@@ -6476,10 +6695,10 @@
         <v>24</v>
       </c>
       <c r="T116" s="23" t="s">
-        <v>199</v>
+        <v>204</v>
       </c>
       <c r="U116" s="23" t="s">
-        <v>185</v>
+        <v>190</v>
       </c>
       <c r="V116" s="0"/>
       <c r="AMJ116" s="0"/>
@@ -6490,7 +6709,7 @@
     </row>
     <row r="118" s="17" customFormat="true" ht="80.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="21" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B118" s="1" t="n">
         <v>96</v>
@@ -6518,7 +6737,7 @@
         <v>44</v>
       </c>
       <c r="J118" s="2" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="K118" s="3"/>
       <c r="L118" s="21" t="n">
@@ -6537,7 +6756,7 @@
         <f aca="false">N118*B118</f>
         <v>358.08</v>
       </c>
-      <c r="Q118" s="54" t="n">
+      <c r="Q118" s="55" t="n">
         <f aca="false">P118-M118</f>
         <v>86.08</v>
       </c>
@@ -6547,15 +6766,12 @@
       </c>
       <c r="S118" s="5"/>
       <c r="T118" s="23" t="s">
-        <v>200</v>
+        <v>205</v>
       </c>
       <c r="U118" s="23" t="s">
-        <v>201</v>
-      </c>
-      <c r="V118" s="0" t="n">
-        <f aca="false">G118</f>
-        <v>0</v>
-      </c>
+        <v>206</v>
+      </c>
+      <c r="V118" s="0"/>
       <c r="AMJ118" s="0"/>
     </row>
     <row r="119" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6564,7 +6780,7 @@
     </row>
     <row r="120" s="17" customFormat="true" ht="106.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="21" t="s">
-        <v>202</v>
+        <v>207</v>
       </c>
       <c r="B120" s="1" t="n">
         <v>96</v>
@@ -6592,7 +6808,7 @@
         <v>44</v>
       </c>
       <c r="J120" s="2" t="s">
-        <v>203</v>
+        <v>208</v>
       </c>
       <c r="K120" s="3"/>
       <c r="L120" s="49" t="n">
@@ -6611,7 +6827,7 @@
         <f aca="false">N120*B120</f>
         <v>358.08</v>
       </c>
-      <c r="Q120" s="54" t="n">
+      <c r="Q120" s="55" t="n">
         <f aca="false">P120-M120</f>
         <v>109.08</v>
       </c>
@@ -6621,15 +6837,12 @@
       </c>
       <c r="S120" s="5"/>
       <c r="T120" s="23" t="s">
-        <v>204</v>
+        <v>209</v>
       </c>
       <c r="U120" s="23" t="s">
-        <v>205</v>
-      </c>
-      <c r="V120" s="0" t="n">
-        <f aca="false">G120</f>
-        <v>0</v>
-      </c>
+        <v>210</v>
+      </c>
+      <c r="V120" s="0"/>
       <c r="AMJ120" s="0"/>
     </row>
     <row r="121" s="17" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6649,7 +6862,7 @@
       <c r="N121" s="1"/>
       <c r="O121" s="1"/>
       <c r="P121" s="1"/>
-      <c r="Q121" s="54"/>
+      <c r="Q121" s="55"/>
       <c r="R121" s="1"/>
       <c r="S121" s="5"/>
       <c r="T121" s="16"/>
@@ -6662,8 +6875,8 @@
       <c r="U122" s="16"/>
     </row>
     <row r="123" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A123" s="61" t="s">
-        <v>206</v>
+      <c r="A123" s="62" t="s">
+        <v>211</v>
       </c>
       <c r="B123" s="1" t="n">
         <v>14</v>
@@ -6687,10 +6900,10 @@
         <v>2</v>
       </c>
       <c r="I123" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="J123" s="62" t="s">
-        <v>207</v>
+        <v>69</v>
+      </c>
+      <c r="J123" s="63" t="s">
+        <v>212</v>
       </c>
       <c r="L123" s="1" t="n">
         <v>47.5</v>
@@ -6708,7 +6921,7 @@
         <f aca="false">N123*B123</f>
         <v>52.22</v>
       </c>
-      <c r="Q123" s="54" t="n">
+      <c r="Q123" s="55" t="n">
         <f aca="false">P123-M123</f>
         <v>24.92</v>
       </c>
@@ -6721,19 +6934,19 @@
         <v>draid2:3d:1s:14c</v>
       </c>
       <c r="U123" s="16" t="s">
-        <v>208</v>
+        <v>213</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J124" s="0" t="s">
-        <v>209</v>
+        <v>214</v>
       </c>
       <c r="T124" s="16"/>
       <c r="U124" s="16"/>
     </row>
     <row r="125" s="17" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A125" s="63" t="s">
-        <v>210</v>
+      <c r="A125" s="64" t="s">
+        <v>215</v>
       </c>
       <c r="B125" s="1" t="n">
         <v>14</v>
@@ -6757,10 +6970,10 @@
         <v>2</v>
       </c>
       <c r="I125" s="2" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="J125" s="17" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="K125" s="3"/>
       <c r="L125" s="1" t="n">
@@ -6779,7 +6992,7 @@
         <f aca="false">N125*B125</f>
         <v>52.22</v>
       </c>
-      <c r="Q125" s="55" t="n">
+      <c r="Q125" s="56" t="n">
         <f aca="false">P125-M125</f>
         <v>14.42</v>
       </c>
@@ -6793,13 +7006,13 @@
         <v>draid2:11d:1s:14c</v>
       </c>
       <c r="U125" s="16" t="s">
-        <v>208</v>
+        <v>213</v>
       </c>
       <c r="V125" s="0"/>
       <c r="AMJ125" s="0"/>
     </row>
     <row r="126" s="17" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A126" s="63"/>
+      <c r="A126" s="64"/>
       <c r="B126" s="1"/>
       <c r="C126" s="1"/>
       <c r="D126" s="1"/>
@@ -6814,7 +7027,7 @@
       <c r="N126" s="1"/>
       <c r="O126" s="1"/>
       <c r="P126" s="1"/>
-      <c r="Q126" s="55"/>
+      <c r="Q126" s="56"/>
       <c r="R126" s="1"/>
       <c r="S126" s="5"/>
       <c r="T126" s="16"/>
@@ -6823,7 +7036,7 @@
       <c r="AMJ126" s="0"/>
     </row>
     <row r="127" s="17" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A127" s="63"/>
+      <c r="A127" s="64"/>
       <c r="B127" s="1"/>
       <c r="C127" s="1"/>
       <c r="D127" s="1"/>
@@ -6838,7 +7051,7 @@
       <c r="N127" s="1"/>
       <c r="O127" s="1"/>
       <c r="P127" s="1"/>
-      <c r="Q127" s="55"/>
+      <c r="Q127" s="56"/>
       <c r="R127" s="1"/>
       <c r="S127" s="5"/>
       <c r="T127" s="16"/>
@@ -6847,8 +7060,8 @@
       <c r="AMJ127" s="0"/>
     </row>
     <row r="128" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A128" s="64" t="s">
-        <v>212</v>
+      <c r="A128" s="65" t="s">
+        <v>217</v>
       </c>
       <c r="T128" s="16" t="str">
         <f aca="false">A128</f>
@@ -6856,180 +7069,118 @@
       </c>
       <c r="U128" s="16"/>
     </row>
-    <row r="129" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A129" s="21" t="s">
-        <v>104</v>
+    <row r="129" s="17" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A129" s="66" t="s">
+        <v>218</v>
       </c>
       <c r="B129" s="21" t="n">
-        <v>32</v>
-      </c>
-      <c r="C129" s="32" t="n">
+        <v>8</v>
+      </c>
+      <c r="C129" s="35" t="n">
         <v>1</v>
       </c>
       <c r="D129" s="1" t="n">
         <f aca="false">B129/C129</f>
-        <v>32</v>
+        <v>8</v>
       </c>
       <c r="E129" s="21" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="F129" s="33" t="n">
         <f aca="false">E129*C129</f>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G129" s="21" t="n">
         <v>0</v>
       </c>
-      <c r="H129" s="14" t="n">
-        <v>1</v>
+      <c r="H129" s="27" t="n">
+        <v>2</v>
       </c>
       <c r="I129" s="2" t="s">
-        <v>105</v>
+        <v>124</v>
       </c>
       <c r="J129" s="17" t="s">
-        <v>60</v>
-      </c>
-      <c r="K129" s="17"/>
-      <c r="L129" s="1" t="n">
-        <v>310</v>
-      </c>
+        <v>61</v>
+      </c>
+      <c r="L129" s="32"/>
       <c r="M129" s="1" t="n">
-        <v>275</v>
+        <v>70</v>
       </c>
       <c r="N129" s="50" t="n">
-        <v>11.2</v>
+        <v>14.55</v>
       </c>
       <c r="O129" s="1" t="n">
-        <v>512</v>
+        <v>4096</v>
       </c>
       <c r="P129" s="1" t="n">
         <f aca="false">N129*B129</f>
-        <v>358.4</v>
+        <v>116.4</v>
       </c>
       <c r="Q129" s="18" t="n">
         <f aca="false">P129-M129</f>
-        <v>83.4</v>
+        <v>46.4</v>
       </c>
       <c r="R129" s="49" t="n">
         <f aca="false">B129+G129</f>
-        <v>32</v>
+        <v>8</v>
       </c>
       <c r="S129" s="15" t="s">
         <v>24</v>
       </c>
       <c r="T129" s="16" t="str">
         <f aca="false">A129</f>
-        <v>draid1:27d:32c:4s</v>
+        <v>DRAID2:5d:1s:8c</v>
       </c>
       <c r="U129" s="16" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="130" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A130" s="67"/>
+      <c r="T130" s="16"/>
+      <c r="U130" s="16"/>
+    </row>
+    <row r="131" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A131" s="21" t="s">
         <v>106</v>
-      </c>
-    </row>
-    <row r="130" customFormat="false" ht="27.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A130" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="B130" s="21" t="n">
-        <v>32</v>
-      </c>
-      <c r="C130" s="21" t="n">
-        <v>2</v>
-      </c>
-      <c r="D130" s="1" t="n">
-        <f aca="false">B130/C130</f>
-        <v>16</v>
-      </c>
-      <c r="E130" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="F130" s="33" t="n">
-        <f aca="false">E130*C130</f>
-        <v>4</v>
-      </c>
-      <c r="G130" s="21" t="n">
-        <v>0</v>
-      </c>
-      <c r="H130" s="14" t="n">
-        <v>1</v>
-      </c>
-      <c r="I130" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="J130" s="17"/>
-      <c r="K130" s="17"/>
-      <c r="L130" s="1" t="n">
-        <v>310</v>
-      </c>
-      <c r="M130" s="1" t="n">
-        <v>275</v>
-      </c>
-      <c r="N130" s="1" t="n">
-        <v>11.2</v>
-      </c>
-      <c r="O130" s="1" t="n">
-        <v>512</v>
-      </c>
-      <c r="P130" s="1" t="n">
-        <f aca="false">N130*B130</f>
-        <v>358.4</v>
-      </c>
-      <c r="Q130" s="18" t="n">
-        <f aca="false">P130-M130</f>
-        <v>83.4</v>
-      </c>
-      <c r="R130" s="49" t="n">
-        <f aca="false">B130+G130</f>
-        <v>32</v>
-      </c>
-      <c r="T130" s="16" t="str">
-        <f aca="false">A130</f>
-        <v>draid1:13d:16c:2s</v>
-      </c>
-      <c r="U130" s="23" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="131" customFormat="false" ht="54.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A131" s="45" t="s">
-        <v>110</v>
       </c>
       <c r="B131" s="21" t="n">
         <v>32</v>
       </c>
-      <c r="C131" s="21" t="n">
-        <v>4</v>
+      <c r="C131" s="32" t="n">
+        <v>1</v>
       </c>
       <c r="D131" s="1" t="n">
         <f aca="false">B131/C131</f>
-        <v>8</v>
-      </c>
-      <c r="E131" s="1" t="n">
-        <v>2</v>
+        <v>32</v>
+      </c>
+      <c r="E131" s="21" t="n">
+        <v>4</v>
       </c>
       <c r="F131" s="33" t="n">
         <f aca="false">E131*C131</f>
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="G131" s="21" t="n">
         <v>0</v>
       </c>
-      <c r="H131" s="19" t="n">
+      <c r="H131" s="14" t="n">
         <v>1</v>
       </c>
       <c r="I131" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="J131" s="65" t="s">
-        <v>111</v>
+        <v>107</v>
+      </c>
+      <c r="J131" s="17" t="s">
+        <v>61</v>
       </c>
       <c r="K131" s="17"/>
-      <c r="L131" s="44" t="n">
-        <v>266</v>
-      </c>
-      <c r="M131" s="21" t="n">
-        <v>211</v>
-      </c>
-      <c r="N131" s="1" t="n">
+      <c r="L131" s="1" t="n">
+        <v>310</v>
+      </c>
+      <c r="M131" s="1" t="n">
+        <v>275</v>
+      </c>
+      <c r="N131" s="50" t="n">
         <v>11.2</v>
       </c>
       <c r="O131" s="1" t="n">
@@ -7039,38 +7190,41 @@
         <f aca="false">N131*B131</f>
         <v>358.4</v>
       </c>
-      <c r="Q131" s="4" t="n">
+      <c r="Q131" s="18" t="n">
         <f aca="false">P131-M131</f>
-        <v>147.4</v>
+        <v>83.4</v>
       </c>
       <c r="R131" s="49" t="n">
         <f aca="false">B131+G131</f>
         <v>32</v>
       </c>
+      <c r="S131" s="15" t="s">
+        <v>24</v>
+      </c>
       <c r="T131" s="16" t="str">
         <f aca="false">A131</f>
-        <v>draid1:5d:8c:2s</v>
-      </c>
-      <c r="U131" s="23" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="132" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>draid1:27d:32c:4s</v>
+      </c>
+      <c r="U131" s="16" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="132" customFormat="false" ht="27.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A132" s="1" t="s">
-        <v>114</v>
+        <v>59</v>
       </c>
       <c r="B132" s="21" t="n">
         <v>32</v>
       </c>
-      <c r="C132" s="32" t="n">
-        <v>1</v>
+      <c r="C132" s="21" t="n">
+        <v>2</v>
       </c>
       <c r="D132" s="1" t="n">
         <f aca="false">B132/C132</f>
-        <v>32</v>
-      </c>
-      <c r="E132" s="21" t="n">
-        <v>4</v>
+        <v>16</v>
+      </c>
+      <c r="E132" s="1" t="n">
+        <v>2</v>
       </c>
       <c r="F132" s="33" t="n">
         <f aca="false">E132*C132</f>
@@ -7079,15 +7233,13 @@
       <c r="G132" s="21" t="n">
         <v>0</v>
       </c>
-      <c r="H132" s="50" t="n">
-        <v>2</v>
+      <c r="H132" s="14" t="n">
+        <v>1</v>
       </c>
       <c r="I132" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="J132" s="17" t="s">
-        <v>116</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="J132" s="17"/>
       <c r="K132" s="17"/>
       <c r="L132" s="1" t="n">
         <v>310</v>
@@ -7113,51 +7265,52 @@
         <f aca="false">B132+G132</f>
         <v>32</v>
       </c>
-      <c r="T132" s="16" t="str">
-        <f aca="false">A132</f>
-        <v>draid2:26d:32c:4s</v>
-      </c>
-      <c r="U132" s="16" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="133" customFormat="false" ht="27.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A133" s="1" t="s">
-        <v>117</v>
+      <c r="T132" s="23" t="s">
+        <v>219</v>
+      </c>
+      <c r="U132" s="23" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="133" customFormat="false" ht="54.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A133" s="45" t="s">
+        <v>112</v>
       </c>
       <c r="B133" s="21" t="n">
         <v>32</v>
       </c>
       <c r="C133" s="21" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D133" s="1" t="n">
         <f aca="false">B133/C133</f>
-        <v>16</v>
+        <v>8</v>
       </c>
       <c r="E133" s="1" t="n">
         <v>2</v>
       </c>
       <c r="F133" s="33" t="n">
         <f aca="false">E133*C133</f>
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="G133" s="21" t="n">
         <v>0</v>
       </c>
-      <c r="H133" s="50" t="n">
-        <v>2</v>
+      <c r="H133" s="19" t="n">
+        <v>1</v>
       </c>
       <c r="I133" s="2" t="s">
-        <v>118</v>
-      </c>
-      <c r="J133" s="17"/>
+        <v>44</v>
+      </c>
+      <c r="J133" s="68" t="s">
+        <v>113</v>
+      </c>
       <c r="K133" s="17"/>
-      <c r="L133" s="1" t="n">
-        <v>310</v>
-      </c>
-      <c r="M133" s="45" t="n">
-        <v>250</v>
+      <c r="L133" s="44" t="n">
+        <v>266</v>
+      </c>
+      <c r="M133" s="21" t="n">
+        <v>211</v>
       </c>
       <c r="N133" s="1" t="n">
         <v>11.2</v>
@@ -7169,42 +7322,41 @@
         <f aca="false">N133*B133</f>
         <v>358.4</v>
       </c>
-      <c r="Q133" s="18" t="n">
+      <c r="Q133" s="4" t="n">
         <f aca="false">P133-M133</f>
-        <v>108.4</v>
+        <v>147.4</v>
       </c>
       <c r="R133" s="49" t="n">
         <f aca="false">B133+G133</f>
         <v>32</v>
       </c>
-      <c r="T133" s="16" t="str">
-        <f aca="false">A133</f>
-        <v>draid2:12d:16c:2s</v>
+      <c r="T133" s="23" t="s">
+        <v>220</v>
       </c>
       <c r="U133" s="23" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="134" customFormat="false" ht="54.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A134" s="45" t="s">
-        <v>120</v>
+        <v>115</v>
+      </c>
+    </row>
+    <row r="134" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A134" s="1" t="s">
+        <v>116</v>
       </c>
       <c r="B134" s="21" t="n">
         <v>32</v>
       </c>
-      <c r="C134" s="21" t="n">
-        <v>4</v>
+      <c r="C134" s="32" t="n">
+        <v>1</v>
       </c>
       <c r="D134" s="1" t="n">
         <f aca="false">B134/C134</f>
-        <v>8</v>
-      </c>
-      <c r="E134" s="44" t="n">
-        <v>2</v>
+        <v>32</v>
+      </c>
+      <c r="E134" s="21" t="n">
+        <v>4</v>
       </c>
       <c r="F134" s="33" t="n">
         <f aca="false">E134*C134</f>
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="G134" s="21" t="n">
         <v>0</v>
@@ -7213,17 +7365,17 @@
         <v>2</v>
       </c>
       <c r="I134" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="J134" s="17" t="s">
         <v>118</v>
       </c>
-      <c r="J134" s="65" t="s">
-        <v>111</v>
-      </c>
       <c r="K134" s="17"/>
-      <c r="L134" s="44" t="n">
-        <v>266</v>
-      </c>
-      <c r="M134" s="44" t="n">
-        <v>172</v>
+      <c r="L134" s="1" t="n">
+        <v>310</v>
+      </c>
+      <c r="M134" s="1" t="n">
+        <v>275</v>
       </c>
       <c r="N134" s="1" t="n">
         <v>11.2</v>
@@ -7235,9 +7387,9 @@
         <f aca="false">N134*B134</f>
         <v>358.4</v>
       </c>
-      <c r="Q134" s="4" t="n">
+      <c r="Q134" s="18" t="n">
         <f aca="false">P134-M134</f>
-        <v>186.4</v>
+        <v>83.4</v>
       </c>
       <c r="R134" s="49" t="n">
         <f aca="false">B134+G134</f>
@@ -7245,28 +7397,28 @@
       </c>
       <c r="T134" s="16" t="str">
         <f aca="false">A134</f>
-        <v>draid2:4d:8c:2s</v>
-      </c>
-      <c r="U134" s="23" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="135" s="17" customFormat="true" ht="54.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A135" s="21" t="s">
-        <v>102</v>
+        <v>draid2:26d:32c:4s</v>
+      </c>
+      <c r="U134" s="16" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="135" customFormat="false" ht="27.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A135" s="1" t="s">
+        <v>119</v>
       </c>
       <c r="B135" s="21" t="n">
         <v>32</v>
       </c>
       <c r="C135" s="21" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D135" s="1" t="n">
         <f aca="false">B135/C135</f>
-        <v>8</v>
-      </c>
-      <c r="E135" s="21" t="n">
-        <v>1</v>
+        <v>16</v>
+      </c>
+      <c r="E135" s="1" t="n">
+        <v>2</v>
       </c>
       <c r="F135" s="33" t="n">
         <f aca="false">E135*C135</f>
@@ -7278,17 +7430,16 @@
       <c r="H135" s="50" t="n">
         <v>2</v>
       </c>
-      <c r="I135" s="20" t="s">
-        <v>122</v>
-      </c>
-      <c r="J135" s="17" t="s">
-        <v>123</v>
-      </c>
-      <c r="L135" s="21" t="n">
+      <c r="I135" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="J135" s="17"/>
+      <c r="K135" s="17"/>
+      <c r="L135" s="1" t="n">
         <v>310</v>
       </c>
       <c r="M135" s="45" t="n">
-        <v>211</v>
+        <v>250</v>
       </c>
       <c r="N135" s="1" t="n">
         <v>11.2</v>
@@ -7302,140 +7453,202 @@
       </c>
       <c r="Q135" s="18" t="n">
         <f aca="false">P135-M135</f>
-        <v>147.4</v>
+        <v>108.4</v>
       </c>
       <c r="R135" s="49" t="n">
         <f aca="false">B135+G135</f>
         <v>32</v>
       </c>
-      <c r="S135" s="5"/>
-      <c r="T135" s="16" t="str">
-        <f aca="false">A135</f>
-        <v>draid2:5d:8c:1s</v>
+      <c r="T135" s="23" t="s">
+        <v>221</v>
       </c>
       <c r="U135" s="23" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="136" customFormat="false" ht="54.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A136" s="45" t="s">
+        <v>122</v>
+      </c>
+      <c r="B136" s="21" t="n">
+        <v>32</v>
+      </c>
+      <c r="C136" s="21" t="n">
+        <v>4</v>
+      </c>
+      <c r="D136" s="1" t="n">
+        <f aca="false">B136/C136</f>
+        <v>8</v>
+      </c>
+      <c r="E136" s="44" t="n">
+        <v>2</v>
+      </c>
+      <c r="F136" s="33" t="n">
+        <f aca="false">E136*C136</f>
+        <v>8</v>
+      </c>
+      <c r="G136" s="21" t="n">
+        <v>0</v>
+      </c>
+      <c r="H136" s="50" t="n">
+        <v>2</v>
+      </c>
+      <c r="I136" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="J136" s="68" t="s">
         <v>113</v>
       </c>
-      <c r="V135" s="0"/>
-      <c r="AMJ135" s="0"/>
-    </row>
-    <row r="136" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="T136" s="16"/>
-      <c r="U136" s="16"/>
-    </row>
-    <row r="137" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="T137" s="16"/>
-      <c r="U137" s="16"/>
-    </row>
-    <row r="138" customFormat="false" ht="54.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A138" s="66" t="s">
-        <v>213</v>
-      </c>
+      <c r="K136" s="17"/>
+      <c r="L136" s="44" t="n">
+        <v>266</v>
+      </c>
+      <c r="M136" s="44" t="n">
+        <v>172</v>
+      </c>
+      <c r="N136" s="1" t="n">
+        <v>11.2</v>
+      </c>
+      <c r="O136" s="1" t="n">
+        <v>512</v>
+      </c>
+      <c r="P136" s="1" t="n">
+        <f aca="false">N136*B136</f>
+        <v>358.4</v>
+      </c>
+      <c r="Q136" s="4" t="n">
+        <f aca="false">P136-M136</f>
+        <v>186.4</v>
+      </c>
+      <c r="R136" s="49" t="n">
+        <f aca="false">B136+G136</f>
+        <v>32</v>
+      </c>
+      <c r="T136" s="23" t="s">
+        <v>222</v>
+      </c>
+      <c r="U136" s="23" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="137" s="17" customFormat="true" ht="54.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A137" s="21" t="s">
+        <v>104</v>
+      </c>
+      <c r="B137" s="21" t="n">
+        <v>32</v>
+      </c>
+      <c r="C137" s="21" t="n">
+        <v>4</v>
+      </c>
+      <c r="D137" s="1" t="n">
+        <f aca="false">B137/C137</f>
+        <v>8</v>
+      </c>
+      <c r="E137" s="21" t="n">
+        <v>1</v>
+      </c>
+      <c r="F137" s="33" t="n">
+        <f aca="false">E137*C137</f>
+        <v>4</v>
+      </c>
+      <c r="G137" s="21" t="n">
+        <v>0</v>
+      </c>
+      <c r="H137" s="50" t="n">
+        <v>2</v>
+      </c>
+      <c r="I137" s="20" t="s">
+        <v>124</v>
+      </c>
+      <c r="J137" s="17" t="s">
+        <v>125</v>
+      </c>
+      <c r="L137" s="21" t="n">
+        <v>310</v>
+      </c>
+      <c r="M137" s="45" t="n">
+        <v>211</v>
+      </c>
+      <c r="N137" s="1" t="n">
+        <v>11.2</v>
+      </c>
+      <c r="O137" s="1" t="n">
+        <v>512</v>
+      </c>
+      <c r="P137" s="1" t="n">
+        <f aca="false">N137*B137</f>
+        <v>358.4</v>
+      </c>
+      <c r="Q137" s="18" t="n">
+        <f aca="false">P137-M137</f>
+        <v>147.4</v>
+      </c>
+      <c r="R137" s="49" t="n">
+        <f aca="false">B137+G137</f>
+        <v>32</v>
+      </c>
+      <c r="S137" s="5"/>
+      <c r="T137" s="23" t="s">
+        <v>223</v>
+      </c>
+      <c r="U137" s="23" t="s">
+        <v>115</v>
+      </c>
+      <c r="V137" s="0"/>
+      <c r="AMJ137" s="0"/>
+    </row>
+    <row r="138" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="T138" s="16"/>
-    </row>
-    <row r="139" customFormat="false" ht="166.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A139" s="67" t="s">
-        <v>214</v>
-      </c>
-      <c r="B139" s="1" t="n">
+      <c r="U138" s="16"/>
+    </row>
+    <row r="139" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="T139" s="16"/>
+      <c r="U139" s="16"/>
+    </row>
+    <row r="140" customFormat="false" ht="54.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A140" s="69" t="s">
+        <v>224</v>
+      </c>
+      <c r="T140" s="16"/>
+    </row>
+    <row r="141" customFormat="false" ht="166.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A141" s="70" t="s">
+        <v>225</v>
+      </c>
+      <c r="B141" s="1" t="n">
         <v>18</v>
       </c>
-      <c r="C139" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="D139" s="44" t="s">
-        <v>215</v>
-      </c>
-      <c r="E139" s="1" t="n">
-        <v>2</v>
-      </c>
-      <c r="F139" s="1" t="n">
+      <c r="C141" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="D141" s="44" t="s">
+        <v>226</v>
+      </c>
+      <c r="E141" s="1" t="n">
+        <v>2</v>
+      </c>
+      <c r="F141" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="G139" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="H139" s="32" t="n">
-        <v>1</v>
-      </c>
-      <c r="I139" s="2" t="s">
-        <v>216</v>
-      </c>
-      <c r="J139" s="68" t="s">
-        <v>217</v>
-      </c>
-      <c r="K139" s="17"/>
-      <c r="L139" s="21" t="n">
+      <c r="G141" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="H141" s="32" t="n">
+        <v>1</v>
+      </c>
+      <c r="I141" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="J141" s="71" t="s">
+        <v>228</v>
+      </c>
+      <c r="K141" s="17"/>
+      <c r="L141" s="21" t="n">
         <v>155</v>
       </c>
-      <c r="M139" s="45" t="n">
+      <c r="M141" s="45" t="n">
         <v>127</v>
-      </c>
-      <c r="N139" s="21" t="n">
-        <v>11.2</v>
-      </c>
-      <c r="O139" s="1" t="n">
-        <v>512</v>
-      </c>
-      <c r="P139" s="1" t="n">
-        <f aca="false">N139*B139</f>
-        <v>201.6</v>
-      </c>
-      <c r="Q139" s="18" t="n">
-        <f aca="false">P139-M139</f>
-        <v>74.6</v>
-      </c>
-      <c r="R139" s="49" t="n">
-        <f aca="false">B139+G139</f>
-        <v>19</v>
-      </c>
-      <c r="T139" s="6" t="str">
-        <f aca="false">A139</f>
-        <v>zp=zdraidtest; time zpool create -o autoreplace=on -o autoexpand=on -O atime=off -O compression=lz4 $zp draid1:5d:8'c':2's' sd{b..i} draid1:7d:10'c':2's' sd{j..s} spare sdt</v>
-      </c>
-    </row>
-    <row r="140" customFormat="false" ht="23.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D140" s="21"/>
-      <c r="I140" s="2" t="s">
-        <v>218</v>
-      </c>
-    </row>
-    <row r="141" customFormat="false" ht="190.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A141" s="67" t="s">
-        <v>219</v>
-      </c>
-      <c r="B141" s="1" t="n">
-        <v>24</v>
-      </c>
-      <c r="C141" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="D141" s="44" t="s">
-        <v>220</v>
-      </c>
-      <c r="E141" s="44" t="s">
-        <v>221</v>
-      </c>
-      <c r="F141" s="1" t="n">
-        <v>5</v>
-      </c>
-      <c r="G141" s="21" t="n">
-        <v>1</v>
-      </c>
-      <c r="H141" s="32" t="n">
-        <v>1</v>
-      </c>
-      <c r="I141" s="2" t="s">
-        <v>222</v>
-      </c>
-      <c r="J141" s="68" t="s">
-        <v>223</v>
-      </c>
-      <c r="L141" s="1" t="n">
-        <v>211</v>
-      </c>
-      <c r="M141" s="1" t="n">
-        <v>170</v>
       </c>
       <c r="N141" s="21" t="n">
         <v>11.2</v>
@@ -7445,78 +7658,126 @@
       </c>
       <c r="P141" s="1" t="n">
         <f aca="false">N141*B141</f>
-        <v>268.8</v>
+        <v>201.6</v>
       </c>
       <c r="Q141" s="18" t="n">
         <f aca="false">P141-M141</f>
-        <v>98.8</v>
+        <v>74.6</v>
       </c>
       <c r="R141" s="49" t="n">
         <f aca="false">B141+G141</f>
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="T141" s="6" t="str">
         <f aca="false">A141</f>
+        <v>zp=zdraidtest; time zpool create -o autoreplace=on -o autoexpand=on -O atime=off -O compression=lz4 $zp draid1:5d:8'c':2's' sd{b..i} draid1:7d:10'c':2's' sd{j..s} spare sdt</v>
+      </c>
+    </row>
+    <row r="142" customFormat="false" ht="23.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D142" s="21"/>
+      <c r="I142" s="2" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="143" customFormat="false" ht="190.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A143" s="70" t="s">
+        <v>230</v>
+      </c>
+      <c r="B143" s="1" t="n">
+        <v>24</v>
+      </c>
+      <c r="C143" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="D143" s="44" t="s">
+        <v>231</v>
+      </c>
+      <c r="E143" s="44" t="s">
+        <v>232</v>
+      </c>
+      <c r="F143" s="1" t="n">
+        <v>5</v>
+      </c>
+      <c r="G143" s="21" t="n">
+        <v>1</v>
+      </c>
+      <c r="H143" s="32" t="n">
+        <v>1</v>
+      </c>
+      <c r="I143" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="J143" s="71" t="s">
+        <v>234</v>
+      </c>
+      <c r="L143" s="1" t="n">
+        <v>211</v>
+      </c>
+      <c r="M143" s="1" t="n">
+        <v>170</v>
+      </c>
+      <c r="N143" s="21" t="n">
+        <v>11.2</v>
+      </c>
+      <c r="O143" s="1" t="n">
+        <v>512</v>
+      </c>
+      <c r="P143" s="1" t="n">
+        <f aca="false">N143*B143</f>
+        <v>268.8</v>
+      </c>
+      <c r="Q143" s="18" t="n">
+        <f aca="false">P143-M143</f>
+        <v>98.8</v>
+      </c>
+      <c r="R143" s="49" t="n">
+        <f aca="false">B143+G143</f>
+        <v>25</v>
+      </c>
+      <c r="T143" s="6" t="str">
+        <f aca="false">A143</f>
         <v>zp=zdraidtest; time zpool create -o autoreplace=on -o autoexpand=on -O atime=off -O compression=lz4 $zp draid1:5d:8'c':2's' sd{b..i} draid1:7d:10'c':2's' sd{j..s} draid1:4d:6'c':1's' sd{t..y} spare sdz</v>
-      </c>
-    </row>
-    <row r="142" customFormat="false" ht="56.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I142" s="2" t="s">
-        <v>224</v>
-      </c>
-      <c r="J142" s="2" t="s">
-        <v>225</v>
-      </c>
-      <c r="K142" s="3" t="n">
-        <v>0.0298611111111111</v>
-      </c>
-      <c r="T142" s="6" t="n">
-        <f aca="false">A142</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="143" customFormat="false" ht="56.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I143" s="2" t="s">
-        <v>226</v>
-      </c>
-      <c r="J143" s="2" t="s">
-        <v>227</v>
-      </c>
-      <c r="K143" s="3" t="n">
-        <v>0.0305555555555556</v>
-      </c>
-      <c r="T143" s="6" t="n">
-        <f aca="false">A143</f>
-        <v>0</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="56.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="I144" s="2" t="s">
-        <v>228</v>
+        <v>235</v>
       </c>
       <c r="J144" s="2" t="s">
-        <v>229</v>
+        <v>236</v>
       </c>
       <c r="K144" s="3" t="n">
-        <v>0.03125</v>
+        <v>0.0298611111111111</v>
       </c>
       <c r="T144" s="6" t="n">
         <f aca="false">A144</f>
         <v>0</v>
       </c>
     </row>
-    <row r="145" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J145" s="0" t="s">
-        <v>230</v>
+    <row r="145" customFormat="false" ht="56.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I145" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="J145" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="K145" s="3" t="n">
+        <v>0.0305555555555556</v>
       </c>
       <c r="T145" s="6" t="n">
         <f aca="false">A145</f>
         <v>0</v>
       </c>
     </row>
-    <row r="146" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J146" s="0" t="s">
-        <v>231</v>
+    <row r="146" customFormat="false" ht="56.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I146" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="J146" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="K146" s="3" t="n">
+        <v>0.03125</v>
       </c>
       <c r="T146" s="6" t="n">
         <f aca="false">A146</f>
@@ -7525,7 +7786,7 @@
     </row>
     <row r="147" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J147" s="0" t="s">
-        <v>232</v>
+        <v>241</v>
       </c>
       <c r="T147" s="6" t="n">
         <f aca="false">A147</f>
@@ -7534,7 +7795,7 @@
     </row>
     <row r="148" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J148" s="0" t="s">
-        <v>233</v>
+        <v>242</v>
       </c>
       <c r="T148" s="6" t="n">
         <f aca="false">A148</f>
@@ -7543,34 +7804,52 @@
     </row>
     <row r="149" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J149" s="0" t="s">
-        <v>234</v>
+        <v>243</v>
       </c>
       <c r="T149" s="6" t="n">
         <f aca="false">A149</f>
         <v>0</v>
       </c>
     </row>
-    <row r="150" customFormat="false" ht="34.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="I150" s="2" t="s">
-        <v>235</v>
-      </c>
+    <row r="150" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="J150" s="0" t="s">
-        <v>236</v>
+        <v>244</v>
       </c>
       <c r="T150" s="6" t="n">
         <f aca="false">A150</f>
         <v>0</v>
       </c>
     </row>
-    <row r="151" customFormat="false" ht="90.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="J151" s="2" t="s">
-        <v>237</v>
-      </c>
-      <c r="K151" s="58" t="n">
-        <v>0.0277777777777778</v>
+    <row r="151" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J151" s="0" t="s">
+        <v>245</v>
       </c>
       <c r="T151" s="6" t="n">
         <f aca="false">A151</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="152" customFormat="false" ht="34.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="I152" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="J152" s="0" t="s">
+        <v>247</v>
+      </c>
+      <c r="T152" s="6" t="n">
+        <f aca="false">A152</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="153" customFormat="false" ht="90.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="J153" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="K153" s="59" t="n">
+        <v>0.0277777777777778</v>
+      </c>
+      <c r="T153" s="6" t="n">
+        <f aca="false">A153</f>
         <v>0</v>
       </c>
     </row>
@@ -7591,123 +7870,192 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D19"/>
+  <dimension ref="A1:E33"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C17" activeCellId="0" sqref="C17"/>
+      <selection pane="topLeft" activeCell="E28" activeCellId="0" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.79"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="57.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="83.27"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="112.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="0" t="s">
-        <v>238</v>
+        <v>249</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>239</v>
+        <v>250</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>240</v>
-      </c>
-      <c r="D1" s="62" t="s">
-        <v>241</v>
+        <v>251</v>
+      </c>
+      <c r="D1" s="63" t="s">
+        <v>252</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C2" s="0" t="s">
-        <v>242</v>
-      </c>
-      <c r="D2" s="0" t="s">
-        <v>243</v>
+        <v>253</v>
+      </c>
+      <c r="D2" s="63" t="s">
+        <v>254</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C4" s="0" t="s">
-        <v>244</v>
-      </c>
-      <c r="D4" s="62" t="s">
-        <v>245</v>
+        <v>255</v>
+      </c>
+      <c r="D4" s="63" t="s">
+        <v>256</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C5" s="0" t="s">
-        <v>246</v>
+        <v>257</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>247</v>
+        <v>258</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C7" s="0" t="s">
-        <v>248</v>
+        <v>259</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>249</v>
+        <v>260</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C8" s="0" t="s">
-        <v>250</v>
+        <v>261</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>251</v>
+        <v>262</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C10" s="62" t="s">
-        <v>252</v>
+      <c r="C10" s="63" t="s">
+        <v>263</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>253</v>
+        <v>264</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C11" s="0" t="s">
-        <v>254</v>
+        <v>265</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C12" s="0" t="s">
-        <v>255</v>
+        <v>266</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>256</v>
+        <v>267</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C14" s="69" t="s">
-        <v>257</v>
+      <c r="C14" s="72" t="s">
+        <v>268</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>209</v>
+        <v>214</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C16" s="0" t="s">
-        <v>258</v>
+        <v>269</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>259</v>
+        <v>270</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C17" s="16" t="s">
-        <v>260</v>
+      <c r="C17" s="73" t="s">
+        <v>271</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D18" s="62" t="s">
-        <v>261</v>
+      <c r="D18" s="63" t="s">
+        <v>272</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C19" s="0" t="s">
+        <v>273</v>
+      </c>
       <c r="D19" s="0" t="s">
-        <v>262</v>
+        <v>274</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C20" s="73" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C21" s="0" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C23" s="74" t="s">
+        <v>277</v>
+      </c>
+      <c r="D23" s="63" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C24" s="0" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C25" s="0" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D27" s="75" t="s">
+        <v>281</v>
+      </c>
+      <c r="E27" s="0" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D28" s="75" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D29" s="75" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D30" s="75" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D31" s="75" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D32" s="75" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D33" s="75" t="s">
+        <v>288</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added non-draid raidz config for 24 drives
</commit_message>
<xml_diff>
--- a/ZFS/zfs-draid-configs.xlsx
+++ b/ZFS/zfs-draid-configs.xlsx
@@ -10,6 +10,7 @@
   <sheets>
     <sheet name="ZFSDRAID" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Notes" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="ZFSnondraid" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -238,8 +239,85 @@
 </comments>
 </file>
 
+<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <authors>
+    <author> </author>
+  </authors>
+  <commentList>
+    <comment ref="E1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Physical disks</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">This is the “free space” in the filesystem you can actually use, can vary with compression</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="L1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">NOTE This is what is seen by the OS as usable space, not HD mfr 1000
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="P1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Total number of physical disks (inpool + spares)</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="R1" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">List of disks to include in VDEV
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="492" uniqueCount="322">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="546" uniqueCount="352">
   <si>
     <t xml:space="preserve">ZFS DRAID configs</t>
   </si>
@@ -1086,6 +1164,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">draid2:10d:30c:1s</t>
     </r>
@@ -1107,6 +1186,7 @@
         <color rgb="FF2FFF12"/>
         <rFont val="Menlo-Regular"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">sdag sdah sdai sdaj sdak sdal sdam sdan sdao sdap sdaq sdar sdas sdat sdau sdav sdaw sdax sdba sdbb sdbc sdbd sdbe sdbf sdbg sdbh sdbi sdbj sdbk sdbl  </t>
     </r>
@@ -1139,6 +1219,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">draid2:7d:10c:1s
 draid2:7d:10c:1s
@@ -1401,15 +1482,120 @@
   <si>
     <t xml:space="preserve">Bold = Standout from other configs, just a point to be aware of, nothing too serious</t>
   </si>
+  <si>
+    <t xml:space="preserve">ZFS RAIDZ configs (non-DRAID)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"># Pspares (per POOL, not per-vdev)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Can sustain X failures PER vdev (Total disks in vdev -raidz level) -pspares, if any</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total time to CP .iso (2.6GB)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lost to parity (GB)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">zp=ztest # Command to create:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">b c d e f g h i j k l m n o p q r s t u v w x y 
+a b c d e f g h i j k l m n o p q r s t u v w x (sdaa sdba sdca)
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">raidz1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 with 2 UNAVAIL and 1 pspare in use</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Insufficient redundancy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.75 sec to lz4; 
+7.55 sec to zstd-3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/dev/sdb /dev/sdc /dev/sdd /dev/sde /dev/sdf /dev/sdg /dev/sdh /dev/sdi /dev/sdj /dev/sdk /dev/sdl /dev/sdm /dev/sdn /dev/sdo /dev/sdp /dev/sdq /dev/sdr /dev/sds /dev/sdt /dev/sdu /dev/sdv /dev/sdw /dev/sdx /dev/sdy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">spare sdz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">raidz2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3 with 3 UNAVAIL and 1 pspare in use</t>
+  </si>
+  <si>
+    <t xml:space="preserve">11.0 sec to lz4; 10.35 sec to zstd-3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">/dev/sd{b..y}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Insufficient hotspares - should have 2-4 at least</t>
+  </si>
+  <si>
+    <t xml:space="preserve">9.4 sec to lz4;
+11.69 sec to zstd-3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">raidz2 /dev/sd{b..m} \
+raidz2 /dev/sd{n..y}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5 with 5 UNAVAIL , 3 pspares in use
+If all pspares are being used the next vdev can only sustain 2 failures</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(Should be) Sufficient hotspares and good redundancy </t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.7 sec to lz4;
+11.55 sec to zstd-3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">raidz2 sdb sdc sdd sde sdf sdg sdh sdi \
+raidz2 sdj sdk sdl sdm sdn sdo sdp sdq \
+raidz2 sdr sds sdt sdu sdv sdw sdx sdy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">spare sdz sdca sdcb </t>
+  </si>
+  <si>
+    <t xml:space="preserve">6 with 6 UNAVAIL , 4 pspares in use; NOTE this is an entire vdev!
+If all pspares are being used the next vdev can only sustain 2 failures</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sufficient hotspares and good redundancy but losing free space to parity; not “wide” enough; however I/O may be faster</t>
+  </si>
+  <si>
+    <t xml:space="preserve">10.6 sec to lz4;
+16.14 sec to zstd-3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">raidz2 sdb sdc sdd sde sdf sdg \
+raidz2 sdh sdi sdj sdk sdl sdm \
+raidz2 sdn sdo sdp sdq sdr sds \
+raidz2 sdt sdu sdv sdw sdx sdy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">spare sdz sdca sdcb sdcc</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="hh:mm"/>
     <numFmt numFmtId="166" formatCode="General"/>
+    <numFmt numFmtId="167" formatCode="#,##0.00"/>
   </numFmts>
   <fonts count="31">
     <font>
@@ -1544,11 +1730,6 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="10.5"/>
       <name val="Courier New"/>
       <family val="3"/>
@@ -1559,6 +1740,7 @@
       <color rgb="FF2FFF12"/>
       <name val="Menlo-Regular"/>
       <family val="0"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -1614,6 +1796,12 @@
       <sz val="12"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Courier New"/>
+      <family val="3"/>
       <charset val="1"/>
     </font>
   </fonts>
@@ -1695,7 +1883,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="81">
+  <cellXfs count="90">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1948,39 +2136,27 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="22" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="23" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="27" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="26" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1992,11 +2168,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2012,12 +2188,60 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="30" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="29" fillId="7" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -2100,12 +2324,12 @@
   <dimension ref="A1:AMJ169"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A147" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A153" activeCellId="0" sqref="A153"/>
+      <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="17.82"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="8.02"/>
@@ -2127,7 +2351,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="5" width="71.56"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="6" width="23.93"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="6" width="65.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="0" width="29.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="0" width="29.56"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="68.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7868,7 +8092,7 @@
       <c r="M150" s="41" t="n">
         <v>107</v>
       </c>
-      <c r="N150" s="63" t="n">
+      <c r="N150" s="1" t="n">
         <v>3.7</v>
       </c>
       <c r="O150" s="1" t="n">
@@ -7893,7 +8117,7 @@
         <f aca="false">A150</f>
         <v>draid2:2d:60c:0s</v>
       </c>
-      <c r="U150" s="64" t="s">
+      <c r="U150" s="23" t="s">
         <v>232</v>
       </c>
     </row>
@@ -7939,7 +8163,7 @@
       <c r="M151" s="40" t="n">
         <v>157</v>
       </c>
-      <c r="N151" s="63" t="n">
+      <c r="N151" s="1" t="n">
         <v>3.7</v>
       </c>
       <c r="O151" s="1" t="n">
@@ -7964,7 +8188,7 @@
         <f aca="false">A151</f>
         <v>draid2:10d:60c:6s</v>
       </c>
-      <c r="U151" s="64" t="s">
+      <c r="U151" s="23" t="s">
         <v>232</v>
       </c>
     </row>
@@ -7975,7 +8199,7 @@
       <c r="B152" s="1" t="n">
         <v>60</v>
       </c>
-      <c r="C152" s="65" t="n">
+      <c r="C152" s="14" t="n">
         <v>2</v>
       </c>
       <c r="D152" s="1" t="n">
@@ -8010,7 +8234,7 @@
       <c r="M152" s="40" t="n">
         <v>157</v>
       </c>
-      <c r="N152" s="63" t="n">
+      <c r="N152" s="1" t="n">
         <v>3.7</v>
       </c>
       <c r="O152" s="1" t="n">
@@ -8034,7 +8258,7 @@
       <c r="T152" s="23" t="s">
         <v>241</v>
       </c>
-      <c r="U152" s="66" t="s">
+      <c r="U152" s="63" t="s">
         <v>242</v>
       </c>
     </row>
@@ -8045,7 +8269,7 @@
       <c r="B153" s="1" t="n">
         <v>60</v>
       </c>
-      <c r="C153" s="65" t="n">
+      <c r="C153" s="14" t="n">
         <v>6</v>
       </c>
       <c r="D153" s="1" t="n">
@@ -8080,7 +8304,7 @@
       <c r="M153" s="40" t="n">
         <v>147</v>
       </c>
-      <c r="N153" s="63" t="n">
+      <c r="N153" s="1" t="n">
         <v>3.7</v>
       </c>
       <c r="O153" s="1" t="n">
@@ -8101,10 +8325,10 @@
       <c r="S153" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="T153" s="66" t="s">
+      <c r="T153" s="63" t="s">
         <v>247</v>
       </c>
-      <c r="U153" s="66" t="s">
+      <c r="U153" s="63" t="s">
         <v>248</v>
       </c>
     </row>
@@ -8117,13 +8341,13 @@
       <c r="U155" s="16"/>
     </row>
     <row r="156" customFormat="false" ht="54.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A156" s="67" t="s">
+      <c r="A156" s="64" t="s">
         <v>249</v>
       </c>
       <c r="T156" s="16"/>
     </row>
     <row r="157" customFormat="false" ht="166.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A157" s="68" t="s">
+      <c r="A157" s="65" t="s">
         <v>250</v>
       </c>
       <c r="B157" s="1" t="n">
@@ -8150,7 +8374,7 @@
       <c r="I157" s="2" t="s">
         <v>252</v>
       </c>
-      <c r="J157" s="69" t="s">
+      <c r="J157" s="66" t="s">
         <v>253</v>
       </c>
       <c r="K157" s="17"/>
@@ -8190,7 +8414,7 @@
       </c>
     </row>
     <row r="159" customFormat="false" ht="190.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A159" s="68" t="s">
+      <c r="A159" s="65" t="s">
         <v>255</v>
       </c>
       <c r="B159" s="1" t="n">
@@ -8217,7 +8441,7 @@
       <c r="I159" s="2" t="s">
         <v>258</v>
       </c>
-      <c r="J159" s="69" t="s">
+      <c r="J159" s="66" t="s">
         <v>259</v>
       </c>
       <c r="L159" s="1" t="n">
@@ -8365,7 +8589,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="J150" r:id="rId2" display="https://zfsonlinux.topicbox.com/groups/zfs-discuss/T5d26c94dbafdb88b"/>
+    <hyperlink ref="J150" r:id="rId2" display="https://zfsonlinux.topicbox.com/groups/zfs-discuss/T5d26c94dbafdb88b – not v.efficient, too much lost to parity and NO vspares"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -8385,15 +8609,15 @@
   </sheetPr>
   <dimension ref="A1:E40"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C22" activeCellId="0" sqref="C22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.79"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="77.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="112.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="112.65"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="20.88"/>
   </cols>
   <sheetData>
@@ -8473,7 +8697,7 @@
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C14" s="70" t="s">
+      <c r="C14" s="67" t="s">
         <v>293</v>
       </c>
       <c r="D14" s="0" t="s">
@@ -8489,7 +8713,7 @@
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C17" s="71" t="s">
+      <c r="C17" s="68" t="s">
         <v>296</v>
       </c>
     </row>
@@ -8507,7 +8731,7 @@
       </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C20" s="71" t="s">
+      <c r="C20" s="68" t="s">
         <v>300</v>
       </c>
     </row>
@@ -8517,7 +8741,7 @@
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C23" s="72" t="s">
+      <c r="C23" s="69" t="s">
         <v>302</v>
       </c>
       <c r="D23" s="55" t="s">
@@ -8525,17 +8749,17 @@
       </c>
     </row>
     <row r="24" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C24" s="73" t="s">
+      <c r="C24" s="70" t="s">
         <v>304</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C25" s="73" t="s">
+      <c r="C25" s="70" t="s">
         <v>305</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D26" s="74" t="s">
+      <c r="D26" s="71" t="s">
         <v>306</v>
       </c>
       <c r="E26" s="0" t="s">
@@ -8543,42 +8767,42 @@
       </c>
     </row>
     <row r="27" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D27" s="75" t="s">
+      <c r="D27" s="72" t="s">
         <v>308</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D28" s="75" t="s">
+      <c r="D28" s="72" t="s">
         <v>309</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D29" s="75" t="s">
+      <c r="D29" s="72" t="s">
         <v>310</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D30" s="75" t="s">
+      <c r="D30" s="72" t="s">
         <v>311</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D31" s="75" t="s">
+      <c r="D31" s="72" t="s">
         <v>312</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D32" s="75" t="s">
+      <c r="D32" s="72" t="s">
         <v>313</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C33" s="76" t="s">
+      <c r="C33" s="73" t="s">
         <v>314</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C34" s="77" t="s">
+      <c r="C34" s="74" t="s">
         <v>315</v>
       </c>
       <c r="D34" s="0" t="s">
@@ -8586,13 +8810,13 @@
       </c>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C35" s="76"/>
+      <c r="C35" s="73"/>
       <c r="D35" s="0" t="s">
         <v>317</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C36" s="78" t="s">
+      <c r="C36" s="75" t="s">
         <v>318</v>
       </c>
       <c r="D36" s="0" t="s">
@@ -8600,15 +8824,15 @@
       </c>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C37" s="76"/>
+      <c r="C37" s="73"/>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C38" s="79" t="s">
+      <c r="C38" s="76" t="s">
         <v>320</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C39" s="80"/>
+      <c r="C39" s="77"/>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C40" s="55" t="s">
@@ -8624,4 +8848,428 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:AMJ6"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="H7" activeCellId="0" sqref="H7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="13.62"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="16.93"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="18.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="29.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="12.47"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="78" customFormat="true" ht="128.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="2" t="s">
+        <v>322</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>323</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>324</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" s="7" t="s">
+        <v>325</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="O1" s="8" t="s">
+        <v>326</v>
+      </c>
+      <c r="P1" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q1" s="9" t="s">
+        <v>327</v>
+      </c>
+      <c r="R1" s="11" t="s">
+        <v>328</v>
+      </c>
+      <c r="S1" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="AMH1" s="0"/>
+      <c r="AMI1" s="0"/>
+      <c r="AMJ1" s="0"/>
+    </row>
+    <row r="2" s="78" customFormat="true" ht="167.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="79" t="s">
+        <v>329</v>
+      </c>
+      <c r="B2" s="2" t="n">
+        <v>24</v>
+      </c>
+      <c r="C2" s="80" t="n">
+        <v>1</v>
+      </c>
+      <c r="D2" s="2" t="n">
+        <v>24</v>
+      </c>
+      <c r="E2" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="F2" s="24" t="n">
+        <v>1</v>
+      </c>
+      <c r="G2" s="31" t="s">
+        <v>330</v>
+      </c>
+      <c r="H2" s="80" t="s">
+        <v>331</v>
+      </c>
+      <c r="I2" s="81" t="s">
+        <v>332</v>
+      </c>
+      <c r="J2" s="2" t="n">
+        <v>89</v>
+      </c>
+      <c r="K2" s="2" t="n">
+        <v>82.4</v>
+      </c>
+      <c r="L2" s="2" t="n">
+        <v>3.73</v>
+      </c>
+      <c r="M2" s="2" t="n">
+        <v>512</v>
+      </c>
+      <c r="N2" s="2" t="n">
+        <f aca="false">L2*B2</f>
+        <v>89.52</v>
+      </c>
+      <c r="O2" s="82" t="n">
+        <f aca="false">N2-K2</f>
+        <v>7.11999999999999</v>
+      </c>
+      <c r="P2" s="2" t="n">
+        <f aca="false">B2+E2</f>
+        <v>25</v>
+      </c>
+      <c r="Q2" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="R2" s="83" t="s">
+        <v>333</v>
+      </c>
+      <c r="S2" s="84" t="s">
+        <v>334</v>
+      </c>
+      <c r="T2" s="12"/>
+      <c r="AMI2" s="0"/>
+      <c r="AMJ2" s="0"/>
+    </row>
+    <row r="3" s="78" customFormat="true" ht="53.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="20" t="s">
+        <v>335</v>
+      </c>
+      <c r="B3" s="2" t="n">
+        <v>24</v>
+      </c>
+      <c r="C3" s="80" t="n">
+        <v>1</v>
+      </c>
+      <c r="D3" s="2" t="n">
+        <v>24</v>
+      </c>
+      <c r="E3" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="F3" s="24" t="n">
+        <v>2</v>
+      </c>
+      <c r="G3" s="31" t="s">
+        <v>336</v>
+      </c>
+      <c r="H3" s="80" t="s">
+        <v>331</v>
+      </c>
+      <c r="I3" s="81" t="s">
+        <v>337</v>
+      </c>
+      <c r="J3" s="2" t="n">
+        <v>89</v>
+      </c>
+      <c r="K3" s="2" t="n">
+        <v>78.1</v>
+      </c>
+      <c r="L3" s="2" t="n">
+        <v>3.73</v>
+      </c>
+      <c r="M3" s="2" t="n">
+        <v>512</v>
+      </c>
+      <c r="N3" s="2" t="n">
+        <f aca="false">L3*B3</f>
+        <v>89.52</v>
+      </c>
+      <c r="O3" s="82" t="n">
+        <f aca="false">N3-K3</f>
+        <v>11.42</v>
+      </c>
+      <c r="P3" s="2" t="n">
+        <f aca="false">B3+E3</f>
+        <v>25</v>
+      </c>
+      <c r="Q3" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="R3" s="83" t="s">
+        <v>338</v>
+      </c>
+      <c r="S3" s="84" t="s">
+        <v>334</v>
+      </c>
+      <c r="T3" s="12"/>
+      <c r="AMI3" s="0"/>
+      <c r="AMJ3" s="0"/>
+    </row>
+    <row r="4" s="78" customFormat="true" ht="53.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="2" t="s">
+        <v>335</v>
+      </c>
+      <c r="B4" s="2" t="n">
+        <v>24</v>
+      </c>
+      <c r="C4" s="85" t="n">
+        <v>2</v>
+      </c>
+      <c r="D4" s="2" t="n">
+        <f aca="false">B4/C4</f>
+        <v>12</v>
+      </c>
+      <c r="E4" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="F4" s="86" t="n">
+        <v>2</v>
+      </c>
+      <c r="G4" s="87" t="s">
+        <v>336</v>
+      </c>
+      <c r="H4" s="88" t="s">
+        <v>339</v>
+      </c>
+      <c r="I4" s="81" t="s">
+        <v>340</v>
+      </c>
+      <c r="J4" s="2" t="n">
+        <v>89</v>
+      </c>
+      <c r="K4" s="2" t="n">
+        <v>71.4</v>
+      </c>
+      <c r="L4" s="2" t="n">
+        <v>3.73</v>
+      </c>
+      <c r="M4" s="2" t="n">
+        <v>512</v>
+      </c>
+      <c r="N4" s="2" t="n">
+        <f aca="false">L4*B4</f>
+        <v>89.52</v>
+      </c>
+      <c r="O4" s="89" t="n">
+        <f aca="false">N4-K4</f>
+        <v>18.12</v>
+      </c>
+      <c r="P4" s="2" t="n">
+        <f aca="false">B4+E4</f>
+        <v>25</v>
+      </c>
+      <c r="Q4" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="R4" s="83" t="s">
+        <v>341</v>
+      </c>
+      <c r="S4" s="84" t="s">
+        <v>334</v>
+      </c>
+      <c r="T4" s="12"/>
+      <c r="AMI4" s="0"/>
+      <c r="AMJ4" s="0"/>
+    </row>
+    <row r="5" s="78" customFormat="true" ht="90.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="2" t="s">
+        <v>335</v>
+      </c>
+      <c r="B5" s="2" t="n">
+        <v>24</v>
+      </c>
+      <c r="C5" s="86" t="n">
+        <v>3</v>
+      </c>
+      <c r="D5" s="2" t="n">
+        <f aca="false">B5/C5</f>
+        <v>8</v>
+      </c>
+      <c r="E5" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="F5" s="86" t="n">
+        <v>2</v>
+      </c>
+      <c r="G5" s="87" t="s">
+        <v>342</v>
+      </c>
+      <c r="H5" s="33" t="s">
+        <v>343</v>
+      </c>
+      <c r="I5" s="81" t="s">
+        <v>344</v>
+      </c>
+      <c r="J5" s="2" t="n">
+        <v>88.5</v>
+      </c>
+      <c r="K5" s="20" t="n">
+        <v>64.1</v>
+      </c>
+      <c r="L5" s="2" t="n">
+        <v>3.73</v>
+      </c>
+      <c r="M5" s="2" t="n">
+        <v>512</v>
+      </c>
+      <c r="N5" s="2" t="n">
+        <f aca="false">L5*B5</f>
+        <v>89.52</v>
+      </c>
+      <c r="O5" s="89" t="n">
+        <f aca="false">N5-K5</f>
+        <v>25.42</v>
+      </c>
+      <c r="P5" s="2" t="n">
+        <f aca="false">B5+E5</f>
+        <v>27</v>
+      </c>
+      <c r="Q5" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="R5" s="83" t="s">
+        <v>345</v>
+      </c>
+      <c r="S5" s="84" t="s">
+        <v>346</v>
+      </c>
+      <c r="T5" s="12"/>
+      <c r="AMI5" s="0"/>
+      <c r="AMJ5" s="0"/>
+    </row>
+    <row r="6" s="78" customFormat="true" ht="134.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="2" t="s">
+        <v>335</v>
+      </c>
+      <c r="B6" s="2" t="n">
+        <v>24</v>
+      </c>
+      <c r="C6" s="86" t="n">
+        <v>4</v>
+      </c>
+      <c r="D6" s="2" t="n">
+        <f aca="false">B6/C6</f>
+        <v>6</v>
+      </c>
+      <c r="E6" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="F6" s="86" t="n">
+        <v>2</v>
+      </c>
+      <c r="G6" s="87" t="s">
+        <v>347</v>
+      </c>
+      <c r="H6" s="86" t="s">
+        <v>348</v>
+      </c>
+      <c r="I6" s="81" t="s">
+        <v>349</v>
+      </c>
+      <c r="J6" s="2" t="n">
+        <v>88</v>
+      </c>
+      <c r="K6" s="2" t="n">
+        <v>56.8</v>
+      </c>
+      <c r="L6" s="2" t="n">
+        <v>3.73</v>
+      </c>
+      <c r="M6" s="2" t="n">
+        <v>512</v>
+      </c>
+      <c r="N6" s="2" t="n">
+        <f aca="false">L6*B6</f>
+        <v>89.52</v>
+      </c>
+      <c r="O6" s="82" t="n">
+        <f aca="false">N6-K6</f>
+        <v>32.72</v>
+      </c>
+      <c r="P6" s="2" t="n">
+        <f aca="false">B6+E6</f>
+        <v>28</v>
+      </c>
+      <c r="Q6" s="15" t="s">
+        <v>24</v>
+      </c>
+      <c r="R6" s="83" t="s">
+        <v>350</v>
+      </c>
+      <c r="S6" s="84" t="s">
+        <v>351</v>
+      </c>
+      <c r="T6" s="12"/>
+      <c r="AMI6" s="0"/>
+      <c r="AMJ6" s="0"/>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>